<commit_message>
Report: Updated Introduction chapter with introduction section
</commit_message>
<xml_diff>
--- a/thesis-fine-grained-classification/binary-relevance/binary-relevance-meka-results.xlsx
+++ b/thesis-fine-grained-classification/binary-relevance/binary-relevance-meka-results.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="232">
   <si>
     <t xml:space="preserve">Model</t>
   </si>
@@ -537,6 +537,18 @@
     <t xml:space="preserve">0.824 0.881 0.940 0.953 0.982</t>
   </si>
   <si>
+    <t xml:space="preserve">0.573 0.393 0.156 0.178 0.735</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.667 0.564 0.471 0.051 0.971</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.413 0.246 0.085 0.099 0.581</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.804 0.861 0.931 0.850 0.982</t>
+  </si>
+  <si>
     <t xml:space="preserve">0.750 0.676 0.427 0.406 0.685</t>
   </si>
   <si>
@@ -561,6 +573,42 @@
     <t xml:space="preserve">0.808 0.879 0.928 0.949 0.976</t>
   </si>
   <si>
+    <t xml:space="preserve">0.448 0.240 0.119 0.039 0.685</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.523 0.566 0.545 0.300 0.968</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.297 0.137 0.063 0.020 0.521</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.760 0.857 0.933 0.944 0.979</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.568 0.366 0.191 0.273 0.768</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.800 0.885 1.000 0.857 0.936</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.402 0.224 0.106 0.158 0.624</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.827 0.881 0.939 0.953 0.982</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.589 0.325 0.091 0.112 0.735</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.656 0.544 0.429 0.375 0.958</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.432 0.195 0.048 0.059 0.581</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.804 0.857 0.931 0.943 0.981</t>
+  </si>
+  <si>
     <t xml:space="preserve">0.766 0.687 0.382 0.430 0.774</t>
   </si>
   <si>
@@ -585,28 +633,91 @@
     <t xml:space="preserve">0.811 0.878 0.938 0.954 0.979</t>
   </si>
   <si>
-    <t xml:space="preserve">0.744 0.719 0.396 0.430 0.691</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.467 0.460 0.388 0.353 0.756</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.786 0.610 0.249 0.276 0.530</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.726 0.837 0.922 0.933 0.973</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.652 0.546 0.217 0.282 0.760</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.647 0.664 0.920 0.893 0.837 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.508 0.380 0.122 0.164 0.615</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.810 0.880 0.940 0.953 0.979</t>
+    <t xml:space="preserve">0.447 0.213 0.110 0.039 0.714</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.513 0.551 0.524 0.333 0.929</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.297 0.120 0.058 0.020 0.556</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.757 0.856 0.932 0.944 0.980</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.551 0.353 0.191 0.282 0.755</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.779 0.917 1.000 0.833 0.934</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.386 0.215 0.106 0.164 0.607</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.821 0.881 0.939 0.953 0.982</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.570 0.390 0.329 0.199 0.721</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.649 0.259 0.129 0.056 0.957</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.412 0.251 0.201 0.112 0.564</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.800 0.784 0.854 0.849 0.981</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.481 0.157 0.165 0.051 0.707</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.540 0.455 0.425 0.333 0.901</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.328 0.085 0.090 0.026 0.547</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.765 0.850 0.930 0.944 0.978</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.555 0.340 0.191 0.282 0.761</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.812 0.933 1.000 0.862 0.923</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.389 0.205 0.106 0.164 0.615</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CV + TFIDF + ngram(1) + stopwords</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.509 0.202 0.081 0.076 0.699</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.556 0.613 0.421 0.857 0.887</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.354 0.112 0.042 0.039 0.538</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.771 0.859 0.931 0.947 0.978</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.643 0.470 0.217 0.292 0.761</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.690 0.676 0.561 0.650 0.911</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.492 0.310 0.122 0.171 0.615</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.820 0.876 0.934 0.950 0.981</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CV + TFIDF + ngram(1) + stopwords + Lemm</t>
   </si>
 </sst>
 </file>
@@ -709,19 +820,19 @@
   </sheetPr>
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.9030612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.4336734693878"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.2448979591837"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.3520408163265"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.5459183673469"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.7959183673469"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.7040816326531"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.0051020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1170,18 +1281,18 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F28" activeCellId="0" sqref="F28"/>
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.8112244897959"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.9438775510204"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.7908163265306"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.9744897959184"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.3418367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.4030612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.25"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.4336734693878"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1625,21 +1736,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F42" activeCellId="0" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.2448979591837"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.7857142857143"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.6785714285714"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="33.6122448979592"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.7040816326531"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.8265306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.9234693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="32.6683673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1862,9 +1973,13 @@
         <v>170</v>
       </c>
     </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+    </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>49</v>
@@ -1884,7 +1999,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>49</v>
@@ -1903,168 +2018,386 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
+      <c r="A17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>186</v>
-      </c>
+        <v>190</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>159</v>
-      </c>
-      <c r="D21" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="E21" s="0" t="s">
-        <v>161</v>
+        <v>58</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>193</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>162</v>
+        <v>194</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="F22" s="0" t="s">
-        <v>166</v>
+      <c r="B23" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>199</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>189</v>
+        <v>205</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>190</v>
+        <v>206</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>191</v>
+        <v>207</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>192</v>
+        <v>208</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>193</v>
+        <v>209</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>194</v>
-      </c>
+        <v>210</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>187</v>
+        <v>211</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>189</v>
+        <v>213</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>190</v>
+        <v>214</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C28" s="0" t="s">
-        <v>191</v>
-      </c>
-      <c r="D28" s="0" t="s">
-        <v>192</v>
-      </c>
-      <c r="E28" s="0" t="s">
-        <v>193</v>
-      </c>
-      <c r="F28" s="0" t="s">
-        <v>194</v>
+      <c r="B29" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="F29" s="0" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="F30" s="0" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F31" s="0" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>224</v>
+      </c>
+      <c r="E36" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="F36" s="0" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>228</v>
+      </c>
+      <c r="E37" s="0" t="s">
+        <v>229</v>
+      </c>
+      <c r="F37" s="0" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>231</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Report: Updated Problem Statement section
</commit_message>
<xml_diff>
--- a/thesis-fine-grained-classification/binary-relevance/binary-relevance-meka-results.xlsx
+++ b/thesis-fine-grained-classification/binary-relevance/binary-relevance-meka-results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Lucene" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="271">
   <si>
     <t xml:space="preserve">Model</t>
   </si>
@@ -357,6 +357,18 @@
     <t xml:space="preserve">0.798 0.869 0.936 0.936 0.982</t>
   </si>
   <si>
+    <t xml:space="preserve">0.397 0.392 0.475 0.439 0.350 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.568 0.575 0.071 0.078 0.739</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.252 0.246 0.589 0.320 0.213</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.773 0.853 0.412 0.669 0.978</t>
+  </si>
+  <si>
     <t xml:space="preserve">0.698 0.622 0.332 0.481 0.570</t>
   </si>
   <si>
@@ -381,6 +393,42 @@
     <t xml:space="preserve">0.793 0.857 0.918 0.923 0.981</t>
   </si>
   <si>
+    <t xml:space="preserve">0.322 0.239 0.026 0.000 0.316</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.512 0.468 0.333 0.000 0.682</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.194 0.136 0.013 0.000 0.188</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.760 0.840 0.926 0.923 0.977</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.385 0.286 0.149 0.246 0.476 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.743 0.844 0.783 0.889 1.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.240 0.167 0.080 0.140 0.313 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.796 0.865 0.932 0.935 0.982</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.387 0.395 0.475 0.497 0.416</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.576 0.580 0.071 0.078 0.750</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.244 0.248 0.589 0.425 0.263</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.773 0.854 0.412 0.586 0.979</t>
+  </si>
+  <si>
     <t xml:space="preserve">0.696 0.665 0.434 0.531 0.556</t>
   </si>
   <si>
@@ -405,28 +453,67 @@
     <t xml:space="preserve">0.794 0.856 0.927 0.921 0.981</t>
   </si>
   <si>
-    <t xml:space="preserve">0.662 0.621 0.367 0.508 0.582</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.483 0.471 0.263 0.359 0.452</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.560 0.473 0.228 0.346 0.413</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.749 0.834 0.898 0.906 0.972</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.582 0.538 0.333 0.409 0.447</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.595 0.550 0.433 0.465 0.920</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.428 0.376 0.201 0.259 0.288</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.791 0.854 0.923 0.923 0.981</t>
+    <t xml:space="preserve">0.318 0.239 0.026 0.000 0.316</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.511 0.468 0.333 0.000 0.682</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.191 0.136 0.013 0.000 0.188</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.374 0.299 0.141 0.253 0.447</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.762 0.876 0.773 0.917 1.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.232 0.176 0.076 0.145 0.288</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.797 0.867 0.931 0.936 0.982</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.469 0.370 0.213 0.512 0.367</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.594 0.534 0.085 0.077 0.692</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.313 0.229 0.121 0.526 0.225</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.782 0.848 0.842 0.500 0.977</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.406 0.252 0.061 0.043 0.280</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.524 0.446 0.438 0.227 1.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.260 0.145 0.031 0.022 0.163</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.764 0.838 0.927 0.922 0.978</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.380 0.316 0.201 0.286 0.462</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.859 0.919 0.806 0.950 1.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.236 0.188 0.112 0.167 0.300</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.806 0.870 0.934 0.938 0.982</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CV + TFIDF + ngram(1) + stopwords</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CV + TFIDF + ngram(1) + stopwords + Lemm</t>
   </si>
   <si>
     <t xml:space="preserve">0.580 0.421 0.363 0.209 0.734</t>
@@ -690,7 +777,40 @@
     <t xml:space="preserve">0.389 0.205 0.106 0.164 0.615</t>
   </si>
   <si>
-    <t xml:space="preserve">CV + TFIDF + ngram(1) + stopwords</t>
+    <t xml:space="preserve">0.486 0.190 0.471 0.297 0.714 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.662 0.581 0.066 0.094 0.890</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.328 0.105 0.587 0.178 0.556</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.793 0.857 0.406 0.862 0.978</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.734 0.704 0.622 0.664 0.730</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.491 0.342 0.187 0.172 0.576</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.710 0.637 0.492 0.546 0.581</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.747 0.766 0.820 0.831 0.964</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.624 0.534 0.333 0.291 0.754</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.646 0.567 0.358 0.333 0.855</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.473 0.371 0.201 0.171 0.607</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.806 0.866 0.921 0.936 0.979</t>
   </si>
   <si>
     <t xml:space="preserve">0.509 0.202 0.081 0.076 0.699</t>
@@ -715,9 +835,6 @@
   </si>
   <si>
     <t xml:space="preserve">0.820 0.876 0.934 0.950 0.981</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CV + TFIDF + ngram(1) + stopwords + Lemm</t>
   </si>
 </sst>
 </file>
@@ -1278,10 +1395,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E33" activeCellId="0" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1515,9 +1632,13 @@
         <v>110</v>
       </c>
     </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+    </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>49</v>
@@ -1537,7 +1658,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>49</v>
@@ -1556,168 +1677,362 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
+      <c r="A17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>126</v>
-      </c>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="D21" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="E21" s="0" t="s">
-        <v>101</v>
+        <v>58</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>133</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>102</v>
+        <v>134</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="F22" s="0" t="s">
-        <v>106</v>
+      <c r="B23" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>127</v>
+        <v>143</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>128</v>
+        <v>144</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>129</v>
+        <v>145</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>131</v>
+        <v>146</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>132</v>
+        <v>147</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>133</v>
+        <v>148</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>134</v>
-      </c>
+        <v>149</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>127</v>
+        <v>150</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>128</v>
+        <v>151</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>129</v>
+        <v>152</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>130</v>
+        <v>153</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C28" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="D28" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="E28" s="0" t="s">
-        <v>133</v>
-      </c>
-      <c r="F28" s="0" t="s">
-        <v>134</v>
+      <c r="B29" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F29" s="0" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="F30" s="0" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="F31" s="0" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -1738,8 +2053,8 @@
   </sheetPr>
   <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F42" activeCellId="0" sqref="F42"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B33" activeCellId="0" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1781,16 +2096,16 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>135</v>
+        <v>164</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>136</v>
+        <v>165</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>137</v>
+        <v>166</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>138</v>
+        <v>167</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1801,16 +2116,16 @@
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>139</v>
+        <v>168</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>140</v>
+        <v>169</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>141</v>
+        <v>170</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>142</v>
+        <v>171</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1821,16 +2136,16 @@
         <v>7</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>143</v>
+        <v>172</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>144</v>
+        <v>173</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>145</v>
+        <v>174</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>146</v>
+        <v>175</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1841,16 +2156,16 @@
         <v>7</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>147</v>
+        <v>176</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>148</v>
+        <v>177</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>149</v>
+        <v>178</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>150</v>
+        <v>179</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1861,16 +2176,16 @@
         <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>151</v>
+        <v>180</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>152</v>
+        <v>181</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>153</v>
+        <v>182</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>154</v>
+        <v>183</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1881,16 +2196,16 @@
         <v>32</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>155</v>
+        <v>184</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>156</v>
+        <v>185</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>157</v>
+        <v>186</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>158</v>
+        <v>187</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1901,16 +2216,16 @@
         <v>32</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>159</v>
+        <v>188</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>160</v>
+        <v>189</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>161</v>
+        <v>190</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>162</v>
+        <v>191</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1921,16 +2236,16 @@
         <v>32</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>163</v>
+        <v>192</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>164</v>
+        <v>193</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>165</v>
+        <v>194</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>166</v>
+        <v>195</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1941,16 +2256,16 @@
         <v>32</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>147</v>
+        <v>176</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>148</v>
+        <v>177</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>149</v>
+        <v>178</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>150</v>
+        <v>179</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1961,16 +2276,16 @@
         <v>32</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>167</v>
+        <v>196</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>168</v>
+        <v>197</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>169</v>
+        <v>198</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>170</v>
+        <v>199</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1985,16 +2300,16 @@
         <v>49</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>171</v>
+        <v>200</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>172</v>
+        <v>201</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>173</v>
+        <v>202</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>174</v>
+        <v>203</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2005,16 +2320,16 @@
         <v>49</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>175</v>
+        <v>204</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>176</v>
+        <v>205</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>177</v>
+        <v>206</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>178</v>
+        <v>207</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2025,16 +2340,16 @@
         <v>49</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>179</v>
+        <v>208</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>180</v>
+        <v>209</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>181</v>
+        <v>210</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>182</v>
+        <v>211</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2045,16 +2360,16 @@
         <v>49</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>183</v>
+        <v>212</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>184</v>
+        <v>213</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>185</v>
+        <v>214</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>186</v>
+        <v>215</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2065,16 +2380,16 @@
         <v>49</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>187</v>
+        <v>216</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>188</v>
+        <v>217</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>189</v>
+        <v>218</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>190</v>
+        <v>219</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2089,16 +2404,16 @@
         <v>58</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>191</v>
+        <v>220</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>192</v>
+        <v>221</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>193</v>
+        <v>222</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>194</v>
+        <v>223</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2109,16 +2424,16 @@
         <v>58</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>195</v>
+        <v>224</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>196</v>
+        <v>225</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>197</v>
+        <v>226</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>198</v>
+        <v>227</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2129,16 +2444,16 @@
         <v>58</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>199</v>
+        <v>228</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>200</v>
+        <v>229</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>201</v>
+        <v>230</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>202</v>
+        <v>231</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2149,16 +2464,16 @@
         <v>58</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>203</v>
+        <v>232</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>204</v>
+        <v>233</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>205</v>
+        <v>234</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>206</v>
+        <v>235</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2169,16 +2484,16 @@
         <v>58</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>207</v>
+        <v>236</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>208</v>
+        <v>237</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>209</v>
+        <v>238</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>210</v>
+        <v>239</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2193,16 +2508,16 @@
         <v>67</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>211</v>
+        <v>240</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>212</v>
+        <v>241</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>213</v>
+        <v>242</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>214</v>
+        <v>243</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2213,16 +2528,16 @@
         <v>67</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>159</v>
+        <v>188</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>160</v>
+        <v>189</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>161</v>
+        <v>190</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>162</v>
+        <v>191</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2233,16 +2548,16 @@
         <v>67</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>163</v>
+        <v>192</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>164</v>
+        <v>193</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>165</v>
+        <v>194</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>166</v>
+        <v>195</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2253,16 +2568,16 @@
         <v>67</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>215</v>
+        <v>244</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>216</v>
+        <v>245</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>217</v>
+        <v>246</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>218</v>
+        <v>247</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2273,16 +2588,16 @@
         <v>67</v>
       </c>
       <c r="C31" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="F31" s="0" t="s">
         <v>219</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="F31" s="0" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2297,7 +2612,19 @@
         <v>6</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>222</v>
+        <v>162</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>251</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>252</v>
+      </c>
+      <c r="E33" s="0" t="s">
+        <v>253</v>
+      </c>
+      <c r="F33" s="0" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2305,7 +2632,19 @@
         <v>12</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>222</v>
+        <v>162</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>255</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>256</v>
+      </c>
+      <c r="E34" s="0" t="s">
+        <v>257</v>
+      </c>
+      <c r="F34" s="0" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2313,7 +2652,19 @@
         <v>17</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>222</v>
+        <v>162</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>259</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>260</v>
+      </c>
+      <c r="E35" s="0" t="s">
+        <v>261</v>
+      </c>
+      <c r="F35" s="0" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2321,19 +2672,19 @@
         <v>22</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>222</v>
+        <v>162</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>223</v>
+        <v>263</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>224</v>
+        <v>264</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>225</v>
+        <v>265</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>226</v>
+        <v>266</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2341,19 +2692,19 @@
         <v>27</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>222</v>
+        <v>162</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>227</v>
+        <v>267</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>228</v>
+        <v>268</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>229</v>
+        <v>269</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>230</v>
+        <v>270</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2365,7 +2716,19 @@
         <v>6</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>231</v>
+        <v>163</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>251</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>252</v>
+      </c>
+      <c r="E39" s="0" t="s">
+        <v>253</v>
+      </c>
+      <c r="F39" s="0" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2373,7 +2736,19 @@
         <v>12</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>231</v>
+        <v>163</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>255</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>256</v>
+      </c>
+      <c r="E40" s="0" t="s">
+        <v>257</v>
+      </c>
+      <c r="F40" s="0" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2381,7 +2756,19 @@
         <v>17</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>231</v>
+        <v>163</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>259</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>260</v>
+      </c>
+      <c r="E41" s="0" t="s">
+        <v>261</v>
+      </c>
+      <c r="F41" s="0" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2389,7 +2776,19 @@
         <v>22</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>231</v>
+        <v>163</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>263</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>264</v>
+      </c>
+      <c r="E42" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="F42" s="0" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2397,7 +2796,19 @@
         <v>27</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>231</v>
+        <v>163</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>267</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>268</v>
+      </c>
+      <c r="E43" s="0" t="s">
+        <v>269</v>
+      </c>
+      <c r="F43" s="0" t="s">
+        <v>270</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated results of Binary Relevance for 5 classifiers, 3 projects, 5 configs
</commit_message>
<xml_diff>
--- a/thesis-fine-grained-classification/binary-relevance/binary-relevance-meka-results.xlsx
+++ b/thesis-fine-grained-classification/binary-relevance/binary-relevance-meka-results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Lucene" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="336">
   <si>
     <t xml:space="preserve">Model</t>
   </si>
@@ -174,6 +174,18 @@
     <t xml:space="preserve">Count Vectorizer + TFIDF + ngram(3)</t>
   </si>
   <si>
+    <t xml:space="preserve">0.501 0.682 0.557 0.368 0.696</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.106 0.680 0.695 0.132 0.854</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.506 0.563 0.394 0.239 0.536</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.497 0.762 0.827 0.729 0.953</t>
+  </si>
+  <si>
     <t xml:space="preserve">0.311 0.747 0.735 0.539 0.816</t>
   </si>
   <si>
@@ -198,9 +210,45 @@
     <t xml:space="preserve">0.883 0.785 0.844 0.886 0.957</t>
   </si>
   <si>
+    <t xml:space="preserve">0.045 0.575 0.494 0.156 0.646 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.545 0.601 0.678 0.421 0.892</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.023 0.434 0.333 0.085 0.478</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.895 0.711 0.817 0.880 0.951</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.182 0.729 0.538 0.284 0.655</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.813 0.761 0.852 0.797 0.935</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.100 0.611 0.370 0.165 0.488</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.902 0.803 0.846 0.898 0.954</t>
+  </si>
+  <si>
     <t xml:space="preserve">Count Vectorizer + TFIDF + ngram(2)</t>
   </si>
   <si>
+    <t xml:space="preserve">0.482 0.667 0.558 0.368 0.699</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.108 0.678 0.704 0.132 0.800</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.614 0.541 0.394 0.239 0.541</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.419 0.758 0.829 0.729 0.950</t>
+  </si>
+  <si>
     <t xml:space="preserve">0.342 0.773 0.742 0.590 0.825</t>
   </si>
   <si>
@@ -225,40 +273,133 @@
     <t xml:space="preserve">0.883 0.792 0.836 0.883 0.959</t>
   </si>
   <si>
+    <t xml:space="preserve">0.074 0.586 0.512 0.156 0.655</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.526 0.615 0.669 0.400 0.894</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.039 0.446 0.350 0.085 0.488 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.895 0.718 0.817 0.879 0.952 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.170 0.739 0.557 0.268 0.689</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.960 0.760 0.858 0.880 0.916</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.093 0.628 0.389 0.155 0.527</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.904 0.807 0.850 0.899 0.956</t>
+  </si>
+  <si>
     <t xml:space="preserve">Count Vectorizer + TFIDF + ngram(1)</t>
   </si>
   <si>
-    <t xml:space="preserve">CV + TFIDF + ngram(3) + stopwords</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.388 0.768 0.729 0.578 0.815</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.423 0.592 0.547 0.356 0.646</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.243 0.854 0.639 0.426 0.705</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.885 0.751 0.803 0.844 0.942</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.374 0.736 0.613 0.420 0.717</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.429 0.744 0.690 0.547 0.928</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.232 0.628 0.455 0.268 0.560</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.886 0.801 0.834 0.889 0.959</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CV + TFIDF + ngram(3) + stopwords + Lemm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.423 0.592 0.547 0.356 0.646 </t>
+    <t xml:space="preserve">0.435 0.656 0.523 0.368 0.715</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.109 0.671 0.674 0.132 0.829</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.317 0.528 0.361 0.239 0.560</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.653 0.753 0.819 0.729 0.953</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.053 0.592 0.499 0.150 0.663</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.412 0.623 0.696 0.426 0.851</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.027 0.452 0.337 0.081 0.498</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.893 0.722 0.820 0.881 0.950 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.170 0.725 0.509 0.263 0.672</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.960 0.772 0.882 0.915 0.946</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.093 0.603 0.343 0.151 0.507</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.904 0.805 0.844 0.900 0.956</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CV + TFIDF + ngram(1) + stopwords</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.275 0.637 0.535 0.473 0.688</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.153 0.658 0.734 0.113 0.838</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.162 0.504 0.370 0.585 0.527</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.816 0.743 0.830 0.419 0.951</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.525 0.739 0.723 0.584 0.860</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.303 0.574 0.450 0.229 0.471</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.371 0.777 0.689 0.461 0.812 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.843 0.729 0.744 0.757 0.907</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.369 0.698 0.662 0.365 0.773</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.428 0.693 0.664 0.432 0.763</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.228 0.583 0.516 0.225 0.638 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.886 0.771 0.834 0.876 0.953</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.067 0.635 0.519 0.035 0.609</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.474 0.630 0.717 0.500 0.813</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.035 0.507 0.355 0.018 0.440</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.894 0.732 0.826 0.884 0.944</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.289 0.721 0.653 0.323 0.775</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.463 0.690 0.699 0.509 0.820 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.170 0.622 0.501 0.194 0.638</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.891 0.778 0.841 0.885 0.957</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CV + TFIDF + ngram(1) + stopwords + Lemm</t>
   </si>
   <si>
     <t xml:space="preserve">0.488 0.410 0.332 0.494 0.416</t>
@@ -510,10 +651,64 @@
     <t xml:space="preserve">0.806 0.870 0.934 0.938 0.982</t>
   </si>
   <si>
-    <t xml:space="preserve">CV + TFIDF + ngram(1) + stopwords</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CV + TFIDF + ngram(1) + stopwords + Lemm</t>
+    <t xml:space="preserve">0.387 0.303 0.332 0.501 0.350</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.578 0.561 0.075 0.074 0.944</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.244 0.180 0.210 0.504 0.213</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.774 0.849 0.755 0.498 0.979</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.668 0.699 0.619 0.605 0.648 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.453 0.393 0.216 0.219 0.145</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.589 0.605 0.482 0.465 0.500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.728 0.791 0.836 0.838 0.911</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.571 0.561 0.333 0.381 0.476</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.580 0.571 0.391 0.432 0.735</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.418 0.399 0.201 0.237 0.313</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.786 0.859 0.919 0.921 0.979</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.413 0.220 0.077 0.009 0.280</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.571 0.488 0.600 0.143 0.929</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.265 0.124 0.040 0.004 0.163</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.774 0.842 0.928 0.924 0.978</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.474 0.500 0.243 0.285 0.431</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.589 0.697 0.525 0.667 0.957</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.319 0.337 0.138 0.167 0.275</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.781 0.873 0.928 0.932 0.981</t>
   </si>
   <si>
     <t xml:space="preserve">0.580 0.421 0.363 0.209 0.734</t>
@@ -935,21 +1130,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C39" activeCellId="0" sqref="C39:F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.7959183673469"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.7040816326531"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.6785714285714"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.0051020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.3928571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.4540816326531"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.4336734693878"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1175,13 +1369,10 @@
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>49</v>
@@ -1201,7 +1392,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>49</v>
@@ -1219,164 +1410,483 @@
         <v>57</v>
       </c>
     </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>61</v>
+      </c>
+    </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>61</v>
+        <v>49</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>65</v>
+        <v>49</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>68</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>66</v>
-      </c>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>37</v>
+        <v>71</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>38</v>
+        <v>72</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>39</v>
+        <v>73</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>40</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C22" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="E22" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="F22" s="0" t="s">
-        <v>44</v>
+      <c r="B23" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>76</v>
-      </c>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>69</v>
+        <v>92</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>71</v>
+        <v>94</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>72</v>
+        <v>95</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C28" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="D28" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="E28" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="F28" s="0" t="s">
-        <v>76</v>
+      <c r="B29" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E29" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="F29" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="F30" s="0" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="E31" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="F31" s="0" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="E33" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="F33" s="0" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="E34" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="F34" s="0" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="E35" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="F35" s="0" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="E36" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="F36" s="0" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="E37" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="F37" s="0" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="E39" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="F39" s="0" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="E40" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="F40" s="0" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="E41" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="F41" s="0" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="E42" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="F42" s="0" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="E43" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="F43" s="0" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -1397,19 +1907,18 @@
   </sheetPr>
   <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E33" activeCellId="0" sqref="E33"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C44" activeCellId="1" sqref="C39:F43 C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.3418367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.4030612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.25"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.4336734693878"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.0051020408163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.8010204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.1326530612245"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.6530612244898"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.1632653061224"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1440,16 +1949,16 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>79</v>
+        <v>126</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>80</v>
+        <v>127</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>81</v>
+        <v>128</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>82</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1460,16 +1969,16 @@
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>83</v>
+        <v>130</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>84</v>
+        <v>131</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>85</v>
+        <v>132</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>86</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1480,16 +1989,16 @@
         <v>7</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>87</v>
+        <v>134</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>88</v>
+        <v>135</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>89</v>
+        <v>136</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>90</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1500,16 +2009,16 @@
         <v>7</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>91</v>
+        <v>138</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>92</v>
+        <v>139</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>93</v>
+        <v>140</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>94</v>
+        <v>141</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1520,16 +2029,16 @@
         <v>7</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>91</v>
+        <v>138</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>92</v>
+        <v>139</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>93</v>
+        <v>140</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>94</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1540,16 +2049,16 @@
         <v>32</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>95</v>
+        <v>142</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>96</v>
+        <v>143</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>97</v>
+        <v>144</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>98</v>
+        <v>145</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1560,16 +2069,16 @@
         <v>32</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>99</v>
+        <v>146</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>100</v>
+        <v>147</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>101</v>
+        <v>148</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>102</v>
+        <v>149</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1580,16 +2089,16 @@
         <v>32</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>103</v>
+        <v>150</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>104</v>
+        <v>151</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>105</v>
+        <v>152</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>106</v>
+        <v>153</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1600,16 +2109,16 @@
         <v>32</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>91</v>
+        <v>138</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>92</v>
+        <v>139</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>93</v>
+        <v>140</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>94</v>
+        <v>141</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1620,16 +2129,16 @@
         <v>32</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>107</v>
+        <v>154</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>108</v>
+        <v>155</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>109</v>
+        <v>156</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>110</v>
+        <v>157</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1644,16 +2153,16 @@
         <v>49</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>111</v>
+        <v>158</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>112</v>
+        <v>159</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>113</v>
+        <v>160</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>114</v>
+        <v>161</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1664,16 +2173,16 @@
         <v>49</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>115</v>
+        <v>162</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>116</v>
+        <v>163</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>117</v>
+        <v>164</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>118</v>
+        <v>165</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1684,16 +2193,16 @@
         <v>49</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>119</v>
+        <v>166</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>120</v>
+        <v>167</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>121</v>
+        <v>168</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>122</v>
+        <v>169</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1704,16 +2213,16 @@
         <v>49</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>123</v>
+        <v>170</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>124</v>
+        <v>171</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>125</v>
+        <v>172</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>126</v>
+        <v>173</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1724,16 +2233,16 @@
         <v>49</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>127</v>
+        <v>174</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>128</v>
+        <v>175</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>129</v>
+        <v>176</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>130</v>
+        <v>177</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1745,19 +2254,19 @@
         <v>6</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>131</v>
+        <v>178</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>132</v>
+        <v>179</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>133</v>
+        <v>180</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>134</v>
+        <v>181</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1765,19 +2274,19 @@
         <v>12</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>135</v>
+        <v>182</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>136</v>
+        <v>183</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>137</v>
+        <v>184</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>138</v>
+        <v>185</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1785,19 +2294,19 @@
         <v>17</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>139</v>
+        <v>186</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>140</v>
+        <v>187</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>141</v>
+        <v>188</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>142</v>
+        <v>189</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1805,19 +2314,19 @@
         <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>143</v>
+        <v>190</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>144</v>
+        <v>191</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>145</v>
+        <v>192</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>126</v>
+        <v>173</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1825,19 +2334,19 @@
         <v>27</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>146</v>
+        <v>193</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>147</v>
+        <v>194</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>148</v>
+        <v>195</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>149</v>
+        <v>196</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1849,19 +2358,19 @@
         <v>6</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>67</v>
+        <v>91</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>150</v>
+        <v>197</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>151</v>
+        <v>198</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>152</v>
+        <v>199</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>153</v>
+        <v>200</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1869,19 +2378,19 @@
         <v>12</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>67</v>
+        <v>91</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>99</v>
+        <v>146</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>100</v>
+        <v>147</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>101</v>
+        <v>148</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>102</v>
+        <v>149</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1889,19 +2398,19 @@
         <v>17</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>67</v>
+        <v>91</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>103</v>
+        <v>150</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>104</v>
+        <v>151</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>105</v>
+        <v>152</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>106</v>
+        <v>153</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1909,19 +2418,19 @@
         <v>22</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>67</v>
+        <v>91</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>154</v>
+        <v>201</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>155</v>
+        <v>202</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>156</v>
+        <v>203</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>157</v>
+        <v>204</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1929,19 +2438,19 @@
         <v>27</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>67</v>
+        <v>91</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>158</v>
+        <v>205</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>159</v>
+        <v>206</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>160</v>
+        <v>207</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>161</v>
+        <v>208</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1956,7 +2465,19 @@
         <v>6</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>162</v>
+        <v>104</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>209</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="E33" s="0" t="s">
+        <v>211</v>
+      </c>
+      <c r="F33" s="0" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1964,7 +2485,19 @@
         <v>12</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>162</v>
+        <v>104</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>214</v>
+      </c>
+      <c r="E34" s="0" t="s">
+        <v>215</v>
+      </c>
+      <c r="F34" s="0" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1972,7 +2505,19 @@
         <v>17</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>162</v>
+        <v>104</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="E35" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F35" s="0" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1980,7 +2525,19 @@
         <v>22</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>162</v>
+        <v>104</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>222</v>
+      </c>
+      <c r="E36" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="F36" s="0" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1988,7 +2545,19 @@
         <v>27</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>162</v>
+        <v>104</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>226</v>
+      </c>
+      <c r="E37" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="F37" s="0" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2000,7 +2569,19 @@
         <v>6</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>163</v>
+        <v>125</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>209</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="E39" s="0" t="s">
+        <v>211</v>
+      </c>
+      <c r="F39" s="0" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2008,7 +2589,19 @@
         <v>12</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>163</v>
+        <v>125</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>214</v>
+      </c>
+      <c r="E40" s="0" t="s">
+        <v>215</v>
+      </c>
+      <c r="F40" s="0" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2016,7 +2609,19 @@
         <v>17</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>163</v>
+        <v>125</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="E41" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F41" s="0" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2024,7 +2629,19 @@
         <v>22</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>163</v>
+        <v>125</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>222</v>
+      </c>
+      <c r="E42" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="F42" s="0" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2032,7 +2649,19 @@
         <v>27</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>163</v>
+        <v>125</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>226</v>
+      </c>
+      <c r="E43" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="F43" s="0" t="s">
+        <v>228</v>
       </c>
     </row>
   </sheetData>
@@ -2053,19 +2682,18 @@
   </sheetPr>
   <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B33" activeCellId="0" sqref="B33"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B33" activeCellId="1" sqref="C39:F43 B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.7040816326531"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.8265306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.9234693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.1071428571429"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="32.6683673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.4336734693878"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.4234693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="32.265306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2096,16 +2724,16 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>164</v>
+        <v>229</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>165</v>
+        <v>230</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>166</v>
+        <v>231</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>167</v>
+        <v>232</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2116,16 +2744,16 @@
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>168</v>
+        <v>233</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>169</v>
+        <v>234</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>170</v>
+        <v>235</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>171</v>
+        <v>236</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2136,16 +2764,16 @@
         <v>7</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>172</v>
+        <v>237</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>173</v>
+        <v>238</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>174</v>
+        <v>239</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>175</v>
+        <v>240</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2156,16 +2784,16 @@
         <v>7</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>176</v>
+        <v>241</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>177</v>
+        <v>242</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>178</v>
+        <v>243</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>179</v>
+        <v>244</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2176,16 +2804,16 @@
         <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>180</v>
+        <v>245</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>181</v>
+        <v>246</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>182</v>
+        <v>247</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>183</v>
+        <v>248</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2196,16 +2824,16 @@
         <v>32</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>184</v>
+        <v>249</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>185</v>
+        <v>250</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>186</v>
+        <v>251</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>187</v>
+        <v>252</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2216,16 +2844,16 @@
         <v>32</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>188</v>
+        <v>253</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>189</v>
+        <v>254</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>190</v>
+        <v>255</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>191</v>
+        <v>256</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2236,16 +2864,16 @@
         <v>32</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>192</v>
+        <v>257</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>193</v>
+        <v>258</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>194</v>
+        <v>259</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>195</v>
+        <v>260</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2256,16 +2884,16 @@
         <v>32</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>176</v>
+        <v>241</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>177</v>
+        <v>242</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>178</v>
+        <v>243</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>179</v>
+        <v>244</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2276,16 +2904,16 @@
         <v>32</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>196</v>
+        <v>261</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>197</v>
+        <v>262</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>198</v>
+        <v>263</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>199</v>
+        <v>264</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2300,16 +2928,16 @@
         <v>49</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>200</v>
+        <v>265</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>201</v>
+        <v>266</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>202</v>
+        <v>267</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>203</v>
+        <v>268</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2320,16 +2948,16 @@
         <v>49</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>204</v>
+        <v>269</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>205</v>
+        <v>270</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>206</v>
+        <v>271</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>207</v>
+        <v>272</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2340,16 +2968,16 @@
         <v>49</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>208</v>
+        <v>273</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>209</v>
+        <v>274</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>210</v>
+        <v>275</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>211</v>
+        <v>276</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2360,16 +2988,16 @@
         <v>49</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>212</v>
+        <v>277</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>213</v>
+        <v>278</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>214</v>
+        <v>279</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>215</v>
+        <v>280</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2380,16 +3008,16 @@
         <v>49</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>216</v>
+        <v>281</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>217</v>
+        <v>282</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>218</v>
+        <v>283</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>219</v>
+        <v>284</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2401,19 +3029,19 @@
         <v>6</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>220</v>
+        <v>285</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>221</v>
+        <v>286</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>222</v>
+        <v>287</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>223</v>
+        <v>288</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2421,19 +3049,19 @@
         <v>12</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>224</v>
+        <v>289</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>225</v>
+        <v>290</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>226</v>
+        <v>291</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>227</v>
+        <v>292</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2441,19 +3069,19 @@
         <v>17</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>228</v>
+        <v>293</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>229</v>
+        <v>294</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>230</v>
+        <v>295</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>231</v>
+        <v>296</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2461,19 +3089,19 @@
         <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>232</v>
+        <v>297</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>233</v>
+        <v>298</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>234</v>
+        <v>299</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>235</v>
+        <v>300</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2481,19 +3109,19 @@
         <v>27</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>236</v>
+        <v>301</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>237</v>
+        <v>302</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>238</v>
+        <v>303</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>239</v>
+        <v>304</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2505,19 +3133,19 @@
         <v>6</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>67</v>
+        <v>91</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>240</v>
+        <v>305</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>241</v>
+        <v>306</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>242</v>
+        <v>307</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>243</v>
+        <v>308</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2525,19 +3153,19 @@
         <v>12</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>67</v>
+        <v>91</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>188</v>
+        <v>253</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>189</v>
+        <v>254</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>190</v>
+        <v>255</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>191</v>
+        <v>256</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2545,19 +3173,19 @@
         <v>17</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>67</v>
+        <v>91</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>192</v>
+        <v>257</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>193</v>
+        <v>258</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>194</v>
+        <v>259</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>195</v>
+        <v>260</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2565,19 +3193,19 @@
         <v>22</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>67</v>
+        <v>91</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>244</v>
+        <v>309</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>245</v>
+        <v>310</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>246</v>
+        <v>311</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>247</v>
+        <v>312</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2585,19 +3213,19 @@
         <v>27</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>67</v>
+        <v>91</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>248</v>
+        <v>313</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>249</v>
+        <v>314</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>250</v>
+        <v>315</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>219</v>
+        <v>284</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2612,19 +3240,19 @@
         <v>6</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>162</v>
+        <v>104</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>251</v>
+        <v>316</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>252</v>
+        <v>317</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>253</v>
+        <v>318</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>254</v>
+        <v>319</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2632,19 +3260,19 @@
         <v>12</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>162</v>
+        <v>104</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>255</v>
+        <v>320</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>256</v>
+        <v>321</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>257</v>
+        <v>322</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>258</v>
+        <v>323</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2652,19 +3280,19 @@
         <v>17</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>162</v>
+        <v>104</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>259</v>
+        <v>324</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>260</v>
+        <v>325</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>261</v>
+        <v>326</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>262</v>
+        <v>327</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2672,19 +3300,19 @@
         <v>22</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>162</v>
+        <v>104</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>263</v>
+        <v>328</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>264</v>
+        <v>329</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>265</v>
+        <v>330</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>266</v>
+        <v>331</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2692,19 +3320,19 @@
         <v>27</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>162</v>
+        <v>104</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>267</v>
+        <v>332</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>268</v>
+        <v>333</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>269</v>
+        <v>334</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>270</v>
+        <v>335</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2716,19 +3344,19 @@
         <v>6</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>163</v>
+        <v>125</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>251</v>
+        <v>316</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>252</v>
+        <v>317</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>253</v>
+        <v>318</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>254</v>
+        <v>319</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2736,19 +3364,19 @@
         <v>12</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>163</v>
+        <v>125</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>255</v>
+        <v>320</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>256</v>
+        <v>321</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>257</v>
+        <v>322</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>258</v>
+        <v>323</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2756,19 +3384,19 @@
         <v>17</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>163</v>
+        <v>125</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>259</v>
+        <v>324</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>260</v>
+        <v>325</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>261</v>
+        <v>326</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>262</v>
+        <v>327</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2776,19 +3404,19 @@
         <v>22</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>163</v>
+        <v>125</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>263</v>
+        <v>328</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>264</v>
+        <v>329</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>265</v>
+        <v>330</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>266</v>
+        <v>331</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2796,19 +3424,19 @@
         <v>27</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>163</v>
+        <v>125</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>267</v>
+        <v>332</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>268</v>
+        <v>333</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>269</v>
+        <v>334</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>270</v>
+        <v>335</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Report: Updated Abstract - English
</commit_message>
<xml_diff>
--- a/thesis-fine-grained-classification/binary-relevance/binary-relevance-meka-results.xlsx
+++ b/thesis-fine-grained-classification/binary-relevance/binary-relevance-meka-results.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="375">
   <si>
     <t xml:space="preserve">Model</t>
   </si>
@@ -400,6 +400,123 @@
   </si>
   <si>
     <t xml:space="preserve">CV + TFIDF + ngram(1) + stopwords + Lemm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Count Vectorizer + TFIDF + ngram(3) + POS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.505 0.660 0.509 0.480 0.679</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.108 0.671 0.704 0.137 0.823</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.510 0.533 0.346 0.366 0.517</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.501 0.753 0.823 0.659 0.950</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.535 0.624 0.640 0.683 0.795</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.258 0.473 0.335 0.209 0.474 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.386 0.926 0.875 0.754 0.696</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.818 0.625 0.587 0.640 0.909</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.367 0.697 0.641 0.432 0.728</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.324 0.656 0.619 0.346 0.702 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.228 0.595 0.494 0.282 0.580 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.868 0.758 0.820 0.855 0.944 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.074 0.625 0.498 0.156 0.599</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.435 0.627 0.658 0.462 0.767</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.039 0.494 0.337 0.085 0.430</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.893 0.729 0.814 0.882 0.941</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.176 0.727 0.536 0.284 0.664</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.893 0.732 0.870 0.810 0.928</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.097 0.617 0.368 0.165 0.498 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.903 0.794 0.848 0.899 0.954</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Count Vectorizer + TFIDF + ngram(2) + POS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.505 0.676 0.477 0.480 0.663</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.108 0.686 0.714 0.137 0.837</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.510 0.552 0.317 0.366 0.498 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.501 0.763 0.820 0.659 0.949</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.549 0.699 0.704 0.693 0.786</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.265 0.518 0.379 0.226 0.500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.402 0.905 0.831 0.701 0.676</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.818 0.683 0.660 0.686 0.915</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.386 0.708 0.659 0.477 0.739</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.323 0.669 0.625 0.373 0.691</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.243 0.609 0.516 0.320 0.594</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.866 0.766 0.824 0.859 0.943 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.067 0.612 0.515 0.144 0.594</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.474 0.631 0.658 0.468 0.765</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.035 0.476 0.354 0.077 0.425</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.894 0.729 0.816 0.883 0.940</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Count Vectorizer + TFIDF + ngram(1) + POS</t>
   </si>
   <si>
     <t xml:space="preserve">0.488 0.410 0.332 0.494 0.416</t>
@@ -1130,20 +1247,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F43"/>
+  <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C39" activeCellId="0" sqref="C39:F43"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C57" activeCellId="0" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.3928571428571"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.4540816326531"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.4336734693878"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.9897959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.0255102040816"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.1632653061224"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1887,6 +2005,234 @@
       </c>
       <c r="F43" s="0" t="s">
         <v>124</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="E45" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="F45" s="0" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="D46" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="E46" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="F46" s="0" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="D47" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="E47" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="F47" s="0" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="D48" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="E48" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="F48" s="0" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="D49" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="E49" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="F49" s="0" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="D51" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="E51" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="F51" s="0" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C52" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="D52" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="E52" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="F52" s="0" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="D53" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="E53" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="F53" s="0" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="D54" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="E54" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="F54" s="0" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -1905,20 +2251,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F43"/>
+  <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C44" activeCellId="1" sqref="C39:F43 C44"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A45" activeCellId="0" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.0051020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.8010204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.1326530612245"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.6530612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.1632653061224"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.3979591836735"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.7295918367347"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1949,16 +2296,16 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>126</v>
+        <v>165</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>127</v>
+        <v>166</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>128</v>
+        <v>167</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>129</v>
+        <v>168</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1969,16 +2316,16 @@
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>130</v>
+        <v>169</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>131</v>
+        <v>170</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>132</v>
+        <v>171</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>133</v>
+        <v>172</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1989,16 +2336,16 @@
         <v>7</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>134</v>
+        <v>173</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>135</v>
+        <v>174</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>136</v>
+        <v>175</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>137</v>
+        <v>176</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2009,16 +2356,16 @@
         <v>7</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>138</v>
+        <v>177</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>139</v>
+        <v>178</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>140</v>
+        <v>179</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>141</v>
+        <v>180</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2029,16 +2376,16 @@
         <v>7</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>138</v>
+        <v>177</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>139</v>
+        <v>178</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>140</v>
+        <v>179</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>141</v>
+        <v>180</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2049,16 +2396,16 @@
         <v>32</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>142</v>
+        <v>181</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>143</v>
+        <v>182</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>144</v>
+        <v>183</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>145</v>
+        <v>184</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2069,16 +2416,16 @@
         <v>32</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>146</v>
+        <v>185</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>147</v>
+        <v>186</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>148</v>
+        <v>187</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>149</v>
+        <v>188</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2089,16 +2436,16 @@
         <v>32</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>150</v>
+        <v>189</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>151</v>
+        <v>190</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>152</v>
+        <v>191</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>153</v>
+        <v>192</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2109,16 +2456,16 @@
         <v>32</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>138</v>
+        <v>177</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>139</v>
+        <v>178</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>140</v>
+        <v>179</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>141</v>
+        <v>180</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2129,16 +2476,16 @@
         <v>32</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>154</v>
+        <v>193</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>155</v>
+        <v>194</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>156</v>
+        <v>195</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>157</v>
+        <v>196</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2153,16 +2500,16 @@
         <v>49</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>158</v>
+        <v>197</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>159</v>
+        <v>198</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>160</v>
+        <v>199</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>161</v>
+        <v>200</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2173,16 +2520,16 @@
         <v>49</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>162</v>
+        <v>201</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>163</v>
+        <v>202</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>164</v>
+        <v>203</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>165</v>
+        <v>204</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2193,16 +2540,16 @@
         <v>49</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>166</v>
+        <v>205</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>167</v>
+        <v>206</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>168</v>
+        <v>207</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>169</v>
+        <v>208</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2213,16 +2560,16 @@
         <v>49</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>170</v>
+        <v>209</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>171</v>
+        <v>210</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>172</v>
+        <v>211</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>173</v>
+        <v>212</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2233,16 +2580,16 @@
         <v>49</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>174</v>
+        <v>213</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>175</v>
+        <v>214</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>176</v>
+        <v>215</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>177</v>
+        <v>216</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2257,16 +2604,16 @@
         <v>70</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>178</v>
+        <v>217</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>179</v>
+        <v>218</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>180</v>
+        <v>219</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>181</v>
+        <v>220</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2277,16 +2624,16 @@
         <v>70</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>182</v>
+        <v>221</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>183</v>
+        <v>222</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>184</v>
+        <v>223</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>185</v>
+        <v>224</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2297,16 +2644,16 @@
         <v>70</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>186</v>
+        <v>225</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>187</v>
+        <v>226</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>188</v>
+        <v>227</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>189</v>
+        <v>228</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2317,16 +2664,16 @@
         <v>70</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>190</v>
+        <v>229</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>191</v>
+        <v>230</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>192</v>
+        <v>231</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>173</v>
+        <v>212</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2337,16 +2684,16 @@
         <v>70</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>193</v>
+        <v>232</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>194</v>
+        <v>233</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>195</v>
+        <v>234</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>196</v>
+        <v>235</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2361,16 +2708,16 @@
         <v>91</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>197</v>
+        <v>236</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>198</v>
+        <v>237</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>199</v>
+        <v>238</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>200</v>
+        <v>239</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2381,16 +2728,16 @@
         <v>91</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>146</v>
+        <v>185</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>147</v>
+        <v>186</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>148</v>
+        <v>187</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>149</v>
+        <v>188</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2401,16 +2748,16 @@
         <v>91</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>150</v>
+        <v>189</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>151</v>
+        <v>190</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>152</v>
+        <v>191</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>153</v>
+        <v>192</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2421,16 +2768,16 @@
         <v>91</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>201</v>
+        <v>240</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>202</v>
+        <v>241</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>203</v>
+        <v>242</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>204</v>
+        <v>243</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2441,16 +2788,16 @@
         <v>91</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>205</v>
+        <v>244</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>206</v>
+        <v>245</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>207</v>
+        <v>246</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>208</v>
+        <v>247</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2468,16 +2815,16 @@
         <v>104</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>209</v>
+        <v>248</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>210</v>
+        <v>249</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>211</v>
+        <v>250</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>212</v>
+        <v>251</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2488,16 +2835,16 @@
         <v>104</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>213</v>
+        <v>252</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>214</v>
+        <v>253</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>215</v>
+        <v>254</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>216</v>
+        <v>255</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2508,16 +2855,16 @@
         <v>104</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>217</v>
+        <v>256</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>218</v>
+        <v>257</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>219</v>
+        <v>258</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>220</v>
+        <v>259</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2528,16 +2875,16 @@
         <v>104</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>221</v>
+        <v>260</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>222</v>
+        <v>261</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>223</v>
+        <v>262</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>224</v>
+        <v>263</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2548,16 +2895,16 @@
         <v>104</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>225</v>
+        <v>264</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>226</v>
+        <v>265</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>227</v>
+        <v>266</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>228</v>
+        <v>267</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2572,16 +2919,16 @@
         <v>125</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>209</v>
+        <v>248</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>210</v>
+        <v>249</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>211</v>
+        <v>250</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>212</v>
+        <v>251</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2592,16 +2939,16 @@
         <v>125</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>213</v>
+        <v>252</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>214</v>
+        <v>253</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>215</v>
+        <v>254</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>216</v>
+        <v>255</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2612,16 +2959,16 @@
         <v>125</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>217</v>
+        <v>256</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>218</v>
+        <v>257</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>219</v>
+        <v>258</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>220</v>
+        <v>259</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2632,16 +2979,16 @@
         <v>125</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>221</v>
+        <v>260</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>222</v>
+        <v>261</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>223</v>
+        <v>262</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>224</v>
+        <v>263</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2652,16 +2999,136 @@
         <v>125</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>225</v>
+        <v>264</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>226</v>
+        <v>265</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>227</v>
+        <v>266</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>228</v>
+        <v>267</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -2680,20 +3147,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F43"/>
+  <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B33" activeCellId="1" sqref="C39:F43 B33"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C47" activeCellId="0" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.4336734693878"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.4234693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.5408163265306"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="32.265306122449"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.1632653061224"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.0204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.2704081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.8571428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2724,16 +3192,16 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>229</v>
+        <v>268</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>230</v>
+        <v>269</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>231</v>
+        <v>270</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>232</v>
+        <v>271</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2744,16 +3212,16 @@
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>234</v>
+        <v>273</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>235</v>
+        <v>274</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>236</v>
+        <v>275</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2764,16 +3232,16 @@
         <v>7</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>237</v>
+        <v>276</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>238</v>
+        <v>277</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>239</v>
+        <v>278</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>240</v>
+        <v>279</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2784,16 +3252,16 @@
         <v>7</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>241</v>
+        <v>280</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>242</v>
+        <v>281</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>243</v>
+        <v>282</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>244</v>
+        <v>283</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2804,16 +3272,16 @@
         <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>245</v>
+        <v>284</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>246</v>
+        <v>285</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>247</v>
+        <v>286</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>248</v>
+        <v>287</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2824,16 +3292,16 @@
         <v>32</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>249</v>
+        <v>288</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>250</v>
+        <v>289</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>251</v>
+        <v>290</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>252</v>
+        <v>291</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2844,16 +3312,16 @@
         <v>32</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>253</v>
+        <v>292</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>254</v>
+        <v>293</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>255</v>
+        <v>294</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>256</v>
+        <v>295</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2864,16 +3332,16 @@
         <v>32</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>257</v>
+        <v>296</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>258</v>
+        <v>297</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>259</v>
+        <v>298</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>260</v>
+        <v>299</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2884,16 +3352,16 @@
         <v>32</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>241</v>
+        <v>280</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>242</v>
+        <v>281</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>243</v>
+        <v>282</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>244</v>
+        <v>283</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2904,16 +3372,16 @@
         <v>32</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>261</v>
+        <v>300</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>262</v>
+        <v>301</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>263</v>
+        <v>302</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>264</v>
+        <v>303</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2928,16 +3396,16 @@
         <v>49</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>265</v>
+        <v>304</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>266</v>
+        <v>305</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>267</v>
+        <v>306</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>268</v>
+        <v>307</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2948,16 +3416,16 @@
         <v>49</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>269</v>
+        <v>308</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>270</v>
+        <v>309</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>271</v>
+        <v>310</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>272</v>
+        <v>311</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2968,16 +3436,16 @@
         <v>49</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>273</v>
+        <v>312</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>274</v>
+        <v>313</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>275</v>
+        <v>314</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>276</v>
+        <v>315</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2988,16 +3456,16 @@
         <v>49</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>277</v>
+        <v>316</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>278</v>
+        <v>317</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>279</v>
+        <v>318</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>280</v>
+        <v>319</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3008,16 +3476,16 @@
         <v>49</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>281</v>
+        <v>320</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>282</v>
+        <v>321</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>283</v>
+        <v>322</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>284</v>
+        <v>323</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3032,16 +3500,16 @@
         <v>70</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>285</v>
+        <v>324</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>286</v>
+        <v>325</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>287</v>
+        <v>326</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>288</v>
+        <v>327</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3052,16 +3520,16 @@
         <v>70</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>289</v>
+        <v>328</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>290</v>
+        <v>329</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>291</v>
+        <v>330</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>292</v>
+        <v>331</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3072,16 +3540,16 @@
         <v>70</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>293</v>
+        <v>332</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>294</v>
+        <v>333</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>295</v>
+        <v>334</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>296</v>
+        <v>335</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3092,16 +3560,16 @@
         <v>70</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>297</v>
+        <v>336</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>298</v>
+        <v>337</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>299</v>
+        <v>338</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>300</v>
+        <v>339</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3112,16 +3580,16 @@
         <v>70</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>301</v>
+        <v>340</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>302</v>
+        <v>341</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>303</v>
+        <v>342</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>304</v>
+        <v>343</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3136,16 +3604,16 @@
         <v>91</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>305</v>
+        <v>344</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>306</v>
+        <v>345</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>307</v>
+        <v>346</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>308</v>
+        <v>347</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3156,16 +3624,16 @@
         <v>91</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>253</v>
+        <v>292</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>254</v>
+        <v>293</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>255</v>
+        <v>294</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>256</v>
+        <v>295</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3176,16 +3644,16 @@
         <v>91</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>257</v>
+        <v>296</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>258</v>
+        <v>297</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>259</v>
+        <v>298</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>260</v>
+        <v>299</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3196,16 +3664,16 @@
         <v>91</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>309</v>
+        <v>348</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>310</v>
+        <v>349</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>311</v>
+        <v>350</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>312</v>
+        <v>351</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3216,16 +3684,16 @@
         <v>91</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>313</v>
+        <v>352</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>314</v>
+        <v>353</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>315</v>
+        <v>354</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>284</v>
+        <v>323</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3243,16 +3711,16 @@
         <v>104</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>316</v>
+        <v>355</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>317</v>
+        <v>356</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>318</v>
+        <v>357</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>319</v>
+        <v>358</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3263,16 +3731,16 @@
         <v>104</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>320</v>
+        <v>359</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>321</v>
+        <v>360</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>322</v>
+        <v>361</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>323</v>
+        <v>362</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3283,16 +3751,16 @@
         <v>104</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>324</v>
+        <v>363</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>325</v>
+        <v>364</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>326</v>
+        <v>365</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>327</v>
+        <v>366</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3303,16 +3771,16 @@
         <v>104</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>328</v>
+        <v>367</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>329</v>
+        <v>368</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>330</v>
+        <v>369</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>331</v>
+        <v>370</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3323,16 +3791,16 @@
         <v>104</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>332</v>
+        <v>371</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>333</v>
+        <v>372</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>334</v>
+        <v>373</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>335</v>
+        <v>374</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3347,16 +3815,16 @@
         <v>125</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>316</v>
+        <v>355</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>317</v>
+        <v>356</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>318</v>
+        <v>357</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>319</v>
+        <v>358</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3367,16 +3835,16 @@
         <v>125</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>320</v>
+        <v>359</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>321</v>
+        <v>360</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>322</v>
+        <v>361</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>323</v>
+        <v>362</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3387,16 +3855,16 @@
         <v>125</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>324</v>
+        <v>363</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>325</v>
+        <v>364</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>326</v>
+        <v>365</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>327</v>
+        <v>366</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3407,16 +3875,16 @@
         <v>125</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>328</v>
+        <v>367</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>329</v>
+        <v>368</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>330</v>
+        <v>369</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>331</v>
+        <v>370</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3427,16 +3895,136 @@
         <v>125</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>332</v>
+        <v>371</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>333</v>
+        <v>372</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>334</v>
+        <v>373</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>335</v>
+        <v>374</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>164</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added results for fine grained classification Config 6 Binary Relevance Lucene
</commit_message>
<xml_diff>
--- a/thesis-fine-grained-classification/binary-relevance/binary-relevance-meka-results.xlsx
+++ b/thesis-fine-grained-classification/binary-relevance/binary-relevance-meka-results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Lucene" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="399">
   <si>
     <t xml:space="preserve">Model</t>
   </si>
@@ -516,7 +516,79 @@
     <t xml:space="preserve">0.894 0.729 0.816 0.883 0.940</t>
   </si>
   <si>
+    <t xml:space="preserve">0.170 0.728 0.543 0.263 0.664</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.889 0.730 0.857 0.896 0.936</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.093 0.620 0.376 0.151 0.498</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.903 0.794 0.848 0.899 0.955</t>
+  </si>
+  <si>
     <t xml:space="preserve">Count Vectorizer + TFIDF + ngram(1) + POS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.457 0.666 0.494 0.480 0.720 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.118 0.672 0.665 0.137 0.848</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.340 0.541 0.333 0.366 0.565 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.661 0.755 0.815 0.659 0.955</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.495 0.728 0.750 0.664 0.835</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.319 0.549 0.444 0.249 0.546</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.340 0.816 0.783 0.585 0.749</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.853 0.711 0.734 0.747 0.926</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.424 0.718 0.699 0.519 0.779</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.336 0.668 0.633 0.420 0.732 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.274 0.626 0.569 0.359 0.647 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.866 0.768 0.831 0.868 0.950</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.053 0.606 0.486 0.156 0.635</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.636 0.599 0.668 0.453 0.735</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.027 0.475 0.326 0.085 0.469</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.895 0.715 0.814 0.882 0.941</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.163 0.734 0.520 0.268 0.677 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.000 0.752 0.865 0.917 0.955</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.089 0.622 0.354 0.155 0.512 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.904 0.803 0.844 0.900 0.957</t>
   </si>
   <si>
     <t xml:space="preserve">0.488 0.410 0.332 0.494 0.416</t>
@@ -1249,8 +1321,8 @@
   </sheetPr>
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C57" activeCellId="0" sqref="C57"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C63" activeCellId="0" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2194,13 +2266,37 @@
       <c r="B55" s="1" t="s">
         <v>147</v>
       </c>
+      <c r="C55" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="D55" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="E55" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="F55" s="0" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>164</v>
+        <v>168</v>
+      </c>
+      <c r="C57" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="D57" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="E57" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="F57" s="0" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2208,7 +2304,19 @@
         <v>12</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>164</v>
+        <v>168</v>
+      </c>
+      <c r="C58" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="D58" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="E58" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="F58" s="0" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2216,7 +2324,19 @@
         <v>17</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>164</v>
+        <v>168</v>
+      </c>
+      <c r="C59" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="D59" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="E59" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="F59" s="0" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2224,7 +2344,19 @@
         <v>22</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>164</v>
+        <v>168</v>
+      </c>
+      <c r="C60" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="D60" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="E60" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="F60" s="0" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2232,7 +2364,19 @@
         <v>27</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>164</v>
+        <v>168</v>
+      </c>
+      <c r="C61" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="D61" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="E61" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="F61" s="0" t="s">
+        <v>188</v>
       </c>
     </row>
   </sheetData>
@@ -2253,8 +2397,8 @@
   </sheetPr>
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A45" activeCellId="0" sqref="A45"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B49" activeCellId="0" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2296,16 +2440,16 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>165</v>
+        <v>189</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>166</v>
+        <v>190</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>167</v>
+        <v>191</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>168</v>
+        <v>192</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2316,16 +2460,16 @@
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>169</v>
+        <v>193</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>170</v>
+        <v>194</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>171</v>
+        <v>195</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>172</v>
+        <v>196</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2336,16 +2480,16 @@
         <v>7</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>173</v>
+        <v>197</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>174</v>
+        <v>198</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>175</v>
+        <v>199</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>176</v>
+        <v>200</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2356,16 +2500,16 @@
         <v>7</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>177</v>
+        <v>201</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>178</v>
+        <v>202</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>179</v>
+        <v>203</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>180</v>
+        <v>204</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2376,16 +2520,16 @@
         <v>7</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>177</v>
+        <v>201</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>178</v>
+        <v>202</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>179</v>
+        <v>203</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>180</v>
+        <v>204</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2396,16 +2540,16 @@
         <v>32</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>181</v>
+        <v>205</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>182</v>
+        <v>206</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>183</v>
+        <v>207</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>184</v>
+        <v>208</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2416,16 +2560,16 @@
         <v>32</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>185</v>
+        <v>209</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>186</v>
+        <v>210</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>187</v>
+        <v>211</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2436,16 +2580,16 @@
         <v>32</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>189</v>
+        <v>213</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>190</v>
+        <v>214</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2456,16 +2600,16 @@
         <v>32</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>177</v>
+        <v>201</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>178</v>
+        <v>202</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>179</v>
+        <v>203</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>180</v>
+        <v>204</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2476,16 +2620,16 @@
         <v>32</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>194</v>
+        <v>218</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>195</v>
+        <v>219</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>196</v>
+        <v>220</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2500,16 +2644,16 @@
         <v>49</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>197</v>
+        <v>221</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>198</v>
+        <v>222</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>199</v>
+        <v>223</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>200</v>
+        <v>224</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2520,16 +2664,16 @@
         <v>49</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>201</v>
+        <v>225</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>202</v>
+        <v>226</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>203</v>
+        <v>227</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>204</v>
+        <v>228</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2540,16 +2684,16 @@
         <v>49</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>205</v>
+        <v>229</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>206</v>
+        <v>230</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>207</v>
+        <v>231</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>208</v>
+        <v>232</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2560,16 +2704,16 @@
         <v>49</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>209</v>
+        <v>233</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>210</v>
+        <v>234</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>211</v>
+        <v>235</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>212</v>
+        <v>236</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2580,16 +2724,16 @@
         <v>49</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>213</v>
+        <v>237</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>214</v>
+        <v>238</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>215</v>
+        <v>239</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>216</v>
+        <v>240</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2604,16 +2748,16 @@
         <v>70</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>217</v>
+        <v>241</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>218</v>
+        <v>242</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>219</v>
+        <v>243</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>220</v>
+        <v>244</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2624,16 +2768,16 @@
         <v>70</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>221</v>
+        <v>245</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>222</v>
+        <v>246</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>223</v>
+        <v>247</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>224</v>
+        <v>248</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2644,16 +2788,16 @@
         <v>70</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>225</v>
+        <v>249</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>226</v>
+        <v>250</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>227</v>
+        <v>251</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>228</v>
+        <v>252</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2664,16 +2808,16 @@
         <v>70</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>229</v>
+        <v>253</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>230</v>
+        <v>254</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>231</v>
+        <v>255</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>212</v>
+        <v>236</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2684,16 +2828,16 @@
         <v>70</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>232</v>
+        <v>256</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>233</v>
+        <v>257</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>234</v>
+        <v>258</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>235</v>
+        <v>259</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2708,16 +2852,16 @@
         <v>91</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>236</v>
+        <v>260</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>237</v>
+        <v>261</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>238</v>
+        <v>262</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>239</v>
+        <v>263</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2728,16 +2872,16 @@
         <v>91</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>185</v>
+        <v>209</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>186</v>
+        <v>210</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>187</v>
+        <v>211</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2748,16 +2892,16 @@
         <v>91</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>189</v>
+        <v>213</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>190</v>
+        <v>214</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2768,16 +2912,16 @@
         <v>91</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>240</v>
+        <v>264</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>241</v>
+        <v>265</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>242</v>
+        <v>266</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>243</v>
+        <v>267</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2788,16 +2932,16 @@
         <v>91</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>244</v>
+        <v>268</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>245</v>
+        <v>269</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>246</v>
+        <v>270</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>247</v>
+        <v>271</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2815,16 +2959,16 @@
         <v>104</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>248</v>
+        <v>272</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>249</v>
+        <v>273</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>250</v>
+        <v>274</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>251</v>
+        <v>275</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2835,16 +2979,16 @@
         <v>104</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>252</v>
+        <v>276</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>253</v>
+        <v>277</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>254</v>
+        <v>278</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>255</v>
+        <v>279</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2855,16 +2999,16 @@
         <v>104</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>256</v>
+        <v>280</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>257</v>
+        <v>281</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>258</v>
+        <v>282</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>259</v>
+        <v>283</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2875,16 +3019,16 @@
         <v>104</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>260</v>
+        <v>284</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>261</v>
+        <v>285</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>262</v>
+        <v>286</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>263</v>
+        <v>287</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2895,16 +3039,16 @@
         <v>104</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>264</v>
+        <v>288</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>265</v>
+        <v>289</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>266</v>
+        <v>290</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>267</v>
+        <v>291</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2919,16 +3063,16 @@
         <v>125</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>248</v>
+        <v>272</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>249</v>
+        <v>273</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>250</v>
+        <v>274</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>251</v>
+        <v>275</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2939,16 +3083,16 @@
         <v>125</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>252</v>
+        <v>276</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>253</v>
+        <v>277</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>254</v>
+        <v>278</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>255</v>
+        <v>279</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2959,16 +3103,16 @@
         <v>125</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>256</v>
+        <v>280</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>257</v>
+        <v>281</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>258</v>
+        <v>282</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>259</v>
+        <v>283</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2979,16 +3123,16 @@
         <v>125</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>260</v>
+        <v>284</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>261</v>
+        <v>285</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>262</v>
+        <v>286</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>263</v>
+        <v>287</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2999,16 +3143,16 @@
         <v>125</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>264</v>
+        <v>288</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>265</v>
+        <v>289</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>266</v>
+        <v>290</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>267</v>
+        <v>291</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3096,7 +3240,7 @@
         <v>6</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3104,7 +3248,7 @@
         <v>12</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3112,7 +3256,7 @@
         <v>17</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3120,7 +3264,7 @@
         <v>22</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3128,7 +3272,7 @@
         <v>27</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -3192,16 +3336,16 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>268</v>
+        <v>292</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>269</v>
+        <v>293</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>270</v>
+        <v>294</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>271</v>
+        <v>295</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3212,16 +3356,16 @@
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>272</v>
+        <v>296</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>273</v>
+        <v>297</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>274</v>
+        <v>298</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>275</v>
+        <v>299</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3232,16 +3376,16 @@
         <v>7</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>276</v>
+        <v>300</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>277</v>
+        <v>301</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>278</v>
+        <v>302</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>279</v>
+        <v>303</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3252,16 +3396,16 @@
         <v>7</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>280</v>
+        <v>304</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>281</v>
+        <v>305</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>282</v>
+        <v>306</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>283</v>
+        <v>307</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3272,16 +3416,16 @@
         <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>284</v>
+        <v>308</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>285</v>
+        <v>309</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>286</v>
+        <v>310</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>287</v>
+        <v>311</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3292,16 +3436,16 @@
         <v>32</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>288</v>
+        <v>312</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>289</v>
+        <v>313</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>290</v>
+        <v>314</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>291</v>
+        <v>315</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3312,16 +3456,16 @@
         <v>32</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>292</v>
+        <v>316</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>293</v>
+        <v>317</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>294</v>
+        <v>318</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>295</v>
+        <v>319</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3332,16 +3476,16 @@
         <v>32</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>296</v>
+        <v>320</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>297</v>
+        <v>321</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>298</v>
+        <v>322</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3352,16 +3496,16 @@
         <v>32</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>280</v>
+        <v>304</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>281</v>
+        <v>305</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>282</v>
+        <v>306</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>283</v>
+        <v>307</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3372,16 +3516,16 @@
         <v>32</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>300</v>
+        <v>324</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>301</v>
+        <v>325</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>302</v>
+        <v>326</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>303</v>
+        <v>327</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3396,16 +3540,16 @@
         <v>49</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>304</v>
+        <v>328</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>305</v>
+        <v>329</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>306</v>
+        <v>330</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>307</v>
+        <v>331</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3416,16 +3560,16 @@
         <v>49</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>308</v>
+        <v>332</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>309</v>
+        <v>333</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>310</v>
+        <v>334</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>311</v>
+        <v>335</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3436,16 +3580,16 @@
         <v>49</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>312</v>
+        <v>336</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>313</v>
+        <v>337</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>314</v>
+        <v>338</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>315</v>
+        <v>339</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3456,16 +3600,16 @@
         <v>49</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>316</v>
+        <v>340</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>317</v>
+        <v>341</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>318</v>
+        <v>342</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>319</v>
+        <v>343</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3476,16 +3620,16 @@
         <v>49</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>320</v>
+        <v>344</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>321</v>
+        <v>345</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>322</v>
+        <v>346</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>323</v>
+        <v>347</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3500,16 +3644,16 @@
         <v>70</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>324</v>
+        <v>348</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>325</v>
+        <v>349</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>326</v>
+        <v>350</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>327</v>
+        <v>351</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3520,16 +3664,16 @@
         <v>70</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>328</v>
+        <v>352</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>329</v>
+        <v>353</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>330</v>
+        <v>354</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>331</v>
+        <v>355</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3540,16 +3684,16 @@
         <v>70</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>332</v>
+        <v>356</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>333</v>
+        <v>357</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>334</v>
+        <v>358</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>335</v>
+        <v>359</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3560,16 +3704,16 @@
         <v>70</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>336</v>
+        <v>360</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>337</v>
+        <v>361</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>338</v>
+        <v>362</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>339</v>
+        <v>363</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3580,16 +3724,16 @@
         <v>70</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>340</v>
+        <v>364</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>341</v>
+        <v>365</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>342</v>
+        <v>366</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>343</v>
+        <v>367</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3604,16 +3748,16 @@
         <v>91</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>344</v>
+        <v>368</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>345</v>
+        <v>369</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>346</v>
+        <v>370</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>347</v>
+        <v>371</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3624,16 +3768,16 @@
         <v>91</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>292</v>
+        <v>316</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>293</v>
+        <v>317</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>294</v>
+        <v>318</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>295</v>
+        <v>319</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3644,16 +3788,16 @@
         <v>91</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>296</v>
+        <v>320</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>297</v>
+        <v>321</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>298</v>
+        <v>322</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3664,16 +3808,16 @@
         <v>91</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>348</v>
+        <v>372</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>349</v>
+        <v>373</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>350</v>
+        <v>374</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>351</v>
+        <v>375</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3684,16 +3828,16 @@
         <v>91</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>352</v>
+        <v>376</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>353</v>
+        <v>377</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>354</v>
+        <v>378</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>323</v>
+        <v>347</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3711,16 +3855,16 @@
         <v>104</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>355</v>
+        <v>379</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>356</v>
+        <v>380</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>357</v>
+        <v>381</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>358</v>
+        <v>382</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3731,16 +3875,16 @@
         <v>104</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>359</v>
+        <v>383</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>360</v>
+        <v>384</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>361</v>
+        <v>385</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>362</v>
+        <v>386</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3751,16 +3895,16 @@
         <v>104</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>363</v>
+        <v>387</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>364</v>
+        <v>388</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>365</v>
+        <v>389</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>366</v>
+        <v>390</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3771,16 +3915,16 @@
         <v>104</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>367</v>
+        <v>391</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>368</v>
+        <v>392</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>369</v>
+        <v>393</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>370</v>
+        <v>394</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3791,16 +3935,16 @@
         <v>104</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>371</v>
+        <v>395</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>372</v>
+        <v>396</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>373</v>
+        <v>397</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>374</v>
+        <v>398</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3815,16 +3959,16 @@
         <v>125</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>355</v>
+        <v>379</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>356</v>
+        <v>380</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>357</v>
+        <v>381</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>358</v>
+        <v>382</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3835,16 +3979,16 @@
         <v>125</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>359</v>
+        <v>383</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>360</v>
+        <v>384</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>361</v>
+        <v>385</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>362</v>
+        <v>386</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3855,16 +3999,16 @@
         <v>125</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>363</v>
+        <v>387</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>364</v>
+        <v>388</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>365</v>
+        <v>389</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>366</v>
+        <v>390</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3875,16 +4019,16 @@
         <v>125</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>367</v>
+        <v>391</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>368</v>
+        <v>392</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>369</v>
+        <v>393</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>370</v>
+        <v>394</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3895,16 +4039,16 @@
         <v>125</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>371</v>
+        <v>395</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>372</v>
+        <v>396</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>373</v>
+        <v>397</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>374</v>
+        <v>398</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3992,7 +4136,7 @@
         <v>6</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4000,7 +4144,7 @@
         <v>12</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4008,7 +4152,7 @@
         <v>17</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4016,7 +4160,7 @@
         <v>22</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4024,7 +4168,7 @@
         <v>27</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Script update for Lucene LDA Keywords
</commit_message>
<xml_diff>
--- a/thesis-fine-grained-classification/binary-relevance/binary-relevance-meka-results.xlsx
+++ b/thesis-fine-grained-classification/binary-relevance/binary-relevance-meka-results.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="854" uniqueCount="455">
   <si>
     <t xml:space="preserve">Model</t>
   </si>
@@ -898,6 +898,174 @@
   </si>
   <si>
     <t xml:space="preserve">0.781 0.873 0.928 0.932 0.981</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.431 0.343 0.480 0.480 0.384</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.601 0.513 0.073 0.074 0.826</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.280 0.209 0.603 0.601 0.238</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.781 0.845 0.414 0.414 0.979</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.673 0.713 0.655 0.710 0.574</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.403 0.341 0.192 0.202 0.158</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.656 0.674 0.545 0.640 0.413</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.682 0.744 0.800 0.786 0.928</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.588 0.583 0.326 0.408 0.475</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.532 0.547 0.265 0.333 0.403 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.443 0.424 0.196 0.259 0.313 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.771 0.855 0.902 0.907 0.970</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.355 0.286 0.000 0.009 0.280</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.500 0.519 0.000 0.167 0.765</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.220 0.167 0.000 0.004 0.163 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.758 0.845 0.926 0.925 0.977 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.431 0.410 0.423 0.424 0.416</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.584 0.560 0.074 0.075 0.724 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.280 0.260 0.714 0.715 0.263</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.777 0.852 0.331 0.332 0.978</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.670 0.720 0.642 0.701 0.597 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.430 0.367 0.206 0.216 0.160 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.612 0.663 0.518 0.610 0.438</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.710 0.768 0.820 0.808 0.926</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.602 0.595 0.320 0.439 0.489</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.534 0.531 0.239 0.342 0.456</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.459 0.438 0.192 0.285 0.325</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.772 0.851 0.897 0.907 0.972</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.384 0.277 0.000 0.000 0.298 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.523 0.523 0.000 0.000 0.667 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.242 0.161 0.000 0.000 0.175 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.763 0.845 0.927 0.924 0.976</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.341 0.287 0.149 0.253 0.416</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.790 0.920 0.818 0.943 1.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.206 0.167 0.080 0.145 0.263</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.795 0.867 0.932 0.936 0.981 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.479 0.340 0.478 0.322 0.298</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.607 0.532 0.072 0.076 0.737</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.323 0.207 0.598 0.820 0.175 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.785 0.847 0.413 0.246 0.977</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.673 0.703 0.572 0.644 0.611</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.458 0.385 0.195 0.233 0.205</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.594 0.618 0.429 0.513 0.450 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.731 0.785 0.830 0.839 0.940</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.607 0.581 0.301 0.450 0.504</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.555 0.537 0.244 0.372 0.519 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.463 0.421 0.179 0.294 0.338</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.780 0.852 0.900 0.911 0.975</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.387 0.246 0.009 0.034 0.261</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.513 0.523 0.200 0.667 0.800</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.245 0.140 0.004 0.018 0.150</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.761 0.845 0.926 0.927 0.977</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.347 0.296 0.194 0.260 0.416</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.867 0.913 0.800 0.944 1.000 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.210 0.174 0.107 0.149 0.263 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.801 0.868 0.933 0.936 0.981</t>
   </si>
   <si>
     <t xml:space="preserve">0.580 0.421 0.363 0.209 0.734</t>
@@ -1321,8 +1489,8 @@
   </sheetPr>
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C63" activeCellId="0" sqref="C63"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B47" activeCellId="0" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2398,7 +2566,7 @@
   <dimension ref="A1:F61"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B49" activeCellId="0" sqref="B49"/>
+      <selection pane="topLeft" activeCell="C48" activeCellId="0" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -3162,6 +3330,18 @@
       <c r="B45" s="1" t="s">
         <v>126</v>
       </c>
+      <c r="C45" s="0" t="s">
+        <v>292</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>293</v>
+      </c>
+      <c r="E45" s="0" t="s">
+        <v>294</v>
+      </c>
+      <c r="F45" s="0" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
@@ -3170,6 +3350,18 @@
       <c r="B46" s="1" t="s">
         <v>126</v>
       </c>
+      <c r="C46" s="0" t="s">
+        <v>296</v>
+      </c>
+      <c r="D46" s="0" t="s">
+        <v>297</v>
+      </c>
+      <c r="E46" s="0" t="s">
+        <v>298</v>
+      </c>
+      <c r="F46" s="0" t="s">
+        <v>299</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
@@ -3178,6 +3370,18 @@
       <c r="B47" s="1" t="s">
         <v>126</v>
       </c>
+      <c r="C47" s="0" t="s">
+        <v>300</v>
+      </c>
+      <c r="D47" s="0" t="s">
+        <v>301</v>
+      </c>
+      <c r="E47" s="0" t="s">
+        <v>302</v>
+      </c>
+      <c r="F47" s="0" t="s">
+        <v>303</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
@@ -3186,6 +3390,18 @@
       <c r="B48" s="1" t="s">
         <v>126</v>
       </c>
+      <c r="C48" s="0" t="s">
+        <v>304</v>
+      </c>
+      <c r="D48" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="E48" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="F48" s="0" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
@@ -3202,6 +3418,18 @@
       <c r="B51" s="1" t="s">
         <v>147</v>
       </c>
+      <c r="C51" s="0" t="s">
+        <v>308</v>
+      </c>
+      <c r="D51" s="0" t="s">
+        <v>309</v>
+      </c>
+      <c r="E51" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="F51" s="0" t="s">
+        <v>311</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
@@ -3210,6 +3438,18 @@
       <c r="B52" s="1" t="s">
         <v>147</v>
       </c>
+      <c r="C52" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="D52" s="0" t="s">
+        <v>313</v>
+      </c>
+      <c r="E52" s="0" t="s">
+        <v>314</v>
+      </c>
+      <c r="F52" s="0" t="s">
+        <v>315</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
@@ -3218,6 +3458,18 @@
       <c r="B53" s="1" t="s">
         <v>147</v>
       </c>
+      <c r="C53" s="0" t="s">
+        <v>316</v>
+      </c>
+      <c r="D53" s="0" t="s">
+        <v>317</v>
+      </c>
+      <c r="E53" s="0" t="s">
+        <v>318</v>
+      </c>
+      <c r="F53" s="0" t="s">
+        <v>319</v>
+      </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
@@ -3226,6 +3478,18 @@
       <c r="B54" s="1" t="s">
         <v>147</v>
       </c>
+      <c r="C54" s="0" t="s">
+        <v>320</v>
+      </c>
+      <c r="D54" s="0" t="s">
+        <v>321</v>
+      </c>
+      <c r="E54" s="0" t="s">
+        <v>322</v>
+      </c>
+      <c r="F54" s="0" t="s">
+        <v>323</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
@@ -3234,6 +3498,18 @@
       <c r="B55" s="1" t="s">
         <v>147</v>
       </c>
+      <c r="C55" s="0" t="s">
+        <v>324</v>
+      </c>
+      <c r="D55" s="0" t="s">
+        <v>325</v>
+      </c>
+      <c r="E55" s="0" t="s">
+        <v>326</v>
+      </c>
+      <c r="F55" s="0" t="s">
+        <v>327</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
@@ -3242,6 +3518,18 @@
       <c r="B57" s="1" t="s">
         <v>168</v>
       </c>
+      <c r="C57" s="0" t="s">
+        <v>328</v>
+      </c>
+      <c r="D57" s="0" t="s">
+        <v>329</v>
+      </c>
+      <c r="E57" s="0" t="s">
+        <v>330</v>
+      </c>
+      <c r="F57" s="0" t="s">
+        <v>331</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
@@ -3250,6 +3538,18 @@
       <c r="B58" s="1" t="s">
         <v>168</v>
       </c>
+      <c r="C58" s="0" t="s">
+        <v>332</v>
+      </c>
+      <c r="D58" s="0" t="s">
+        <v>333</v>
+      </c>
+      <c r="E58" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="F58" s="0" t="s">
+        <v>335</v>
+      </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
@@ -3258,6 +3558,18 @@
       <c r="B59" s="1" t="s">
         <v>168</v>
       </c>
+      <c r="C59" s="0" t="s">
+        <v>336</v>
+      </c>
+      <c r="D59" s="0" t="s">
+        <v>337</v>
+      </c>
+      <c r="E59" s="0" t="s">
+        <v>338</v>
+      </c>
+      <c r="F59" s="0" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
@@ -3266,6 +3578,18 @@
       <c r="B60" s="1" t="s">
         <v>168</v>
       </c>
+      <c r="C60" s="0" t="s">
+        <v>340</v>
+      </c>
+      <c r="D60" s="0" t="s">
+        <v>341</v>
+      </c>
+      <c r="E60" s="0" t="s">
+        <v>342</v>
+      </c>
+      <c r="F60" s="0" t="s">
+        <v>343</v>
+      </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
@@ -3273,6 +3597,18 @@
       </c>
       <c r="B61" s="1" t="s">
         <v>168</v>
+      </c>
+      <c r="C61" s="0" t="s">
+        <v>344</v>
+      </c>
+      <c r="D61" s="0" t="s">
+        <v>345</v>
+      </c>
+      <c r="E61" s="0" t="s">
+        <v>346</v>
+      </c>
+      <c r="F61" s="0" t="s">
+        <v>347</v>
       </c>
     </row>
   </sheetData>
@@ -3336,16 +3672,16 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>292</v>
+        <v>348</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>293</v>
+        <v>349</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>294</v>
+        <v>350</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>295</v>
+        <v>351</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3356,16 +3692,16 @@
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>296</v>
+        <v>352</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>297</v>
+        <v>353</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>298</v>
+        <v>354</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>299</v>
+        <v>355</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3376,16 +3712,16 @@
         <v>7</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>300</v>
+        <v>356</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>301</v>
+        <v>357</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>302</v>
+        <v>358</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>303</v>
+        <v>359</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3396,16 +3732,16 @@
         <v>7</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>304</v>
+        <v>360</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>305</v>
+        <v>361</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>306</v>
+        <v>362</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>307</v>
+        <v>363</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3416,16 +3752,16 @@
         <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>308</v>
+        <v>364</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>309</v>
+        <v>365</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>310</v>
+        <v>366</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>311</v>
+        <v>367</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3436,16 +3772,16 @@
         <v>32</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>312</v>
+        <v>368</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>313</v>
+        <v>369</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>314</v>
+        <v>370</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>315</v>
+        <v>371</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3456,16 +3792,16 @@
         <v>32</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>316</v>
+        <v>372</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>317</v>
+        <v>373</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>318</v>
+        <v>374</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>319</v>
+        <v>375</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3476,16 +3812,16 @@
         <v>32</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>320</v>
+        <v>376</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>321</v>
+        <v>377</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>322</v>
+        <v>378</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>323</v>
+        <v>379</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3496,16 +3832,16 @@
         <v>32</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>304</v>
+        <v>360</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>305</v>
+        <v>361</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>306</v>
+        <v>362</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>307</v>
+        <v>363</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3516,16 +3852,16 @@
         <v>32</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>324</v>
+        <v>380</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>325</v>
+        <v>381</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>326</v>
+        <v>382</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>327</v>
+        <v>383</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3540,16 +3876,16 @@
         <v>49</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>328</v>
+        <v>384</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>329</v>
+        <v>385</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>330</v>
+        <v>386</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>331</v>
+        <v>387</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3560,16 +3896,16 @@
         <v>49</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>332</v>
+        <v>388</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>333</v>
+        <v>389</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>334</v>
+        <v>390</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>335</v>
+        <v>391</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3580,16 +3916,16 @@
         <v>49</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>336</v>
+        <v>392</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>337</v>
+        <v>393</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>338</v>
+        <v>394</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>339</v>
+        <v>395</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3600,16 +3936,16 @@
         <v>49</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>340</v>
+        <v>396</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>341</v>
+        <v>397</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>342</v>
+        <v>398</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>343</v>
+        <v>399</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3620,16 +3956,16 @@
         <v>49</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>344</v>
+        <v>400</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>345</v>
+        <v>401</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>346</v>
+        <v>402</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>347</v>
+        <v>403</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3644,16 +3980,16 @@
         <v>70</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>348</v>
+        <v>404</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>349</v>
+        <v>405</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>350</v>
+        <v>406</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>351</v>
+        <v>407</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3664,16 +4000,16 @@
         <v>70</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>352</v>
+        <v>408</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>353</v>
+        <v>409</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>354</v>
+        <v>410</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>355</v>
+        <v>411</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3684,16 +4020,16 @@
         <v>70</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>356</v>
+        <v>412</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>357</v>
+        <v>413</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>358</v>
+        <v>414</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>359</v>
+        <v>415</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3704,16 +4040,16 @@
         <v>70</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>360</v>
+        <v>416</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>361</v>
+        <v>417</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>362</v>
+        <v>418</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>363</v>
+        <v>419</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3724,16 +4060,16 @@
         <v>70</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>364</v>
+        <v>420</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>365</v>
+        <v>421</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>366</v>
+        <v>422</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>367</v>
+        <v>423</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3748,16 +4084,16 @@
         <v>91</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>368</v>
+        <v>424</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>369</v>
+        <v>425</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>370</v>
+        <v>426</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>371</v>
+        <v>427</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3768,16 +4104,16 @@
         <v>91</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>316</v>
+        <v>372</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>317</v>
+        <v>373</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>318</v>
+        <v>374</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>319</v>
+        <v>375</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3788,16 +4124,16 @@
         <v>91</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>320</v>
+        <v>376</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>321</v>
+        <v>377</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>322</v>
+        <v>378</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>323</v>
+        <v>379</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3808,16 +4144,16 @@
         <v>91</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>372</v>
+        <v>428</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>373</v>
+        <v>429</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>374</v>
+        <v>430</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>375</v>
+        <v>431</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3828,16 +4164,16 @@
         <v>91</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>376</v>
+        <v>432</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>377</v>
+        <v>433</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>378</v>
+        <v>434</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>347</v>
+        <v>403</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3855,16 +4191,16 @@
         <v>104</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>379</v>
+        <v>435</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>380</v>
+        <v>436</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>381</v>
+        <v>437</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>382</v>
+        <v>438</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3875,16 +4211,16 @@
         <v>104</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>383</v>
+        <v>439</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>384</v>
+        <v>440</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>385</v>
+        <v>441</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>386</v>
+        <v>442</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3895,16 +4231,16 @@
         <v>104</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>387</v>
+        <v>443</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>388</v>
+        <v>444</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>389</v>
+        <v>445</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>390</v>
+        <v>446</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3915,16 +4251,16 @@
         <v>104</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>391</v>
+        <v>447</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>392</v>
+        <v>448</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>393</v>
+        <v>449</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>394</v>
+        <v>450</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3935,16 +4271,16 @@
         <v>104</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>395</v>
+        <v>451</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>396</v>
+        <v>452</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>397</v>
+        <v>453</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>398</v>
+        <v>454</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3959,16 +4295,16 @@
         <v>125</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>379</v>
+        <v>435</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>380</v>
+        <v>436</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>381</v>
+        <v>437</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>382</v>
+        <v>438</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3979,16 +4315,16 @@
         <v>125</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>383</v>
+        <v>439</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>384</v>
+        <v>440</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>385</v>
+        <v>441</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>386</v>
+        <v>442</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3999,16 +4335,16 @@
         <v>125</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>387</v>
+        <v>443</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>388</v>
+        <v>444</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>389</v>
+        <v>445</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>390</v>
+        <v>446</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4019,16 +4355,16 @@
         <v>125</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>391</v>
+        <v>447</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>392</v>
+        <v>448</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>393</v>
+        <v>449</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>394</v>
+        <v>450</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4039,16 +4375,16 @@
         <v>125</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>395</v>
+        <v>451</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>396</v>
+        <v>452</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>397</v>
+        <v>453</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>398</v>
+        <v>454</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Added results for fine grained classification Config 6 Binary Relevance Thunderbird
</commit_message>
<xml_diff>
--- a/thesis-fine-grained-classification/binary-relevance/binary-relevance-meka-results.xlsx
+++ b/thesis-fine-grained-classification/binary-relevance/binary-relevance-meka-results.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="854" uniqueCount="455">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="858" uniqueCount="459">
   <si>
     <t xml:space="preserve">Model</t>
   </si>
@@ -946,6 +946,18 @@
   </si>
   <si>
     <t xml:space="preserve">0.758 0.845 0.926 0.925 0.977 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.332 0.265 0.118 0.259 0.431</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.768 0.871 0.824 0.829 1.000 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.199 0.153 0.063 0.149 0.275</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.792 0.864 0.931 0.935 0.981 </t>
   </si>
   <si>
     <t xml:space="preserve">0.431 0.410 0.423 0.424 0.416</t>
@@ -2566,7 +2578,7 @@
   <dimension ref="A1:F61"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C48" activeCellId="0" sqref="C48"/>
+      <selection pane="topLeft" activeCell="C47" activeCellId="0" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -3410,6 +3422,18 @@
       <c r="B49" s="1" t="s">
         <v>126</v>
       </c>
+      <c r="C49" s="0" t="s">
+        <v>308</v>
+      </c>
+      <c r="D49" s="0" t="s">
+        <v>309</v>
+      </c>
+      <c r="E49" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="F49" s="0" t="s">
+        <v>311</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
@@ -3419,16 +3443,16 @@
         <v>147</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="F51" s="0" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3439,16 +3463,16 @@
         <v>147</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="F52" s="0" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3459,16 +3483,16 @@
         <v>147</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="F53" s="0" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3479,16 +3503,16 @@
         <v>147</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="F54" s="0" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3499,16 +3523,16 @@
         <v>147</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="F55" s="0" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3519,16 +3543,16 @@
         <v>168</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>328</v>
+        <v>332</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="F57" s="0" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3539,16 +3563,16 @@
         <v>168</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="E58" s="0" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="F58" s="0" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3559,16 +3583,16 @@
         <v>168</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="E59" s="0" t="s">
-        <v>338</v>
+        <v>342</v>
       </c>
       <c r="F59" s="0" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3579,16 +3603,16 @@
         <v>168</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>340</v>
+        <v>344</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>341</v>
+        <v>345</v>
       </c>
       <c r="E60" s="0" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="F60" s="0" t="s">
-        <v>343</v>
+        <v>347</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3599,16 +3623,16 @@
         <v>168</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>344</v>
+        <v>348</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>345</v>
+        <v>349</v>
       </c>
       <c r="E61" s="0" t="s">
-        <v>346</v>
+        <v>350</v>
       </c>
       <c r="F61" s="0" t="s">
-        <v>347</v>
+        <v>351</v>
       </c>
     </row>
   </sheetData>
@@ -3672,16 +3696,16 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>349</v>
+        <v>353</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>351</v>
+        <v>355</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3692,16 +3716,16 @@
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>352</v>
+        <v>356</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>353</v>
+        <v>357</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>354</v>
+        <v>358</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>355</v>
+        <v>359</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3712,16 +3736,16 @@
         <v>7</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>356</v>
+        <v>360</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>357</v>
+        <v>361</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>358</v>
+        <v>362</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>359</v>
+        <v>363</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3732,16 +3756,16 @@
         <v>7</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>360</v>
+        <v>364</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>361</v>
+        <v>365</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>362</v>
+        <v>366</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>363</v>
+        <v>367</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3752,16 +3776,16 @@
         <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>364</v>
+        <v>368</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>365</v>
+        <v>369</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>366</v>
+        <v>370</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>367</v>
+        <v>371</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3772,16 +3796,16 @@
         <v>32</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>371</v>
+        <v>375</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3792,16 +3816,16 @@
         <v>32</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>372</v>
+        <v>376</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>373</v>
+        <v>377</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>374</v>
+        <v>378</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>375</v>
+        <v>379</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3812,16 +3836,16 @@
         <v>32</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>376</v>
+        <v>380</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>377</v>
+        <v>381</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>378</v>
+        <v>382</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>379</v>
+        <v>383</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3832,16 +3856,16 @@
         <v>32</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>360</v>
+        <v>364</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>361</v>
+        <v>365</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>362</v>
+        <v>366</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>363</v>
+        <v>367</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3852,16 +3876,16 @@
         <v>32</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>380</v>
+        <v>384</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>381</v>
+        <v>385</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>382</v>
+        <v>386</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>383</v>
+        <v>387</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3876,16 +3900,16 @@
         <v>49</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>384</v>
+        <v>388</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>385</v>
+        <v>389</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>386</v>
+        <v>390</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>387</v>
+        <v>391</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3896,16 +3920,16 @@
         <v>49</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>388</v>
+        <v>392</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>391</v>
+        <v>395</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3916,16 +3940,16 @@
         <v>49</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>392</v>
+        <v>396</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>394</v>
+        <v>398</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3936,16 +3960,16 @@
         <v>49</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>396</v>
+        <v>400</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>397</v>
+        <v>401</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>398</v>
+        <v>402</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>399</v>
+        <v>403</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3956,16 +3980,16 @@
         <v>49</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>401</v>
+        <v>405</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>402</v>
+        <v>406</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>403</v>
+        <v>407</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3980,16 +4004,16 @@
         <v>70</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>404</v>
+        <v>408</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>405</v>
+        <v>409</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>406</v>
+        <v>410</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>407</v>
+        <v>411</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4000,16 +4024,16 @@
         <v>70</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>408</v>
+        <v>412</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>409</v>
+        <v>413</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>410</v>
+        <v>414</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>411</v>
+        <v>415</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4020,16 +4044,16 @@
         <v>70</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>412</v>
+        <v>416</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>413</v>
+        <v>417</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>414</v>
+        <v>418</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>415</v>
+        <v>419</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4040,16 +4064,16 @@
         <v>70</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>416</v>
+        <v>420</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>417</v>
+        <v>421</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>418</v>
+        <v>422</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>419</v>
+        <v>423</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4060,16 +4084,16 @@
         <v>70</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>421</v>
+        <v>425</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>422</v>
+        <v>426</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4084,16 +4108,16 @@
         <v>91</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>424</v>
+        <v>428</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>425</v>
+        <v>429</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>426</v>
+        <v>430</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4104,16 +4128,16 @@
         <v>91</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>372</v>
+        <v>376</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>373</v>
+        <v>377</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>374</v>
+        <v>378</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>375</v>
+        <v>379</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4124,16 +4148,16 @@
         <v>91</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>376</v>
+        <v>380</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>377</v>
+        <v>381</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>378</v>
+        <v>382</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>379</v>
+        <v>383</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4144,16 +4168,16 @@
         <v>91</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>428</v>
+        <v>432</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>429</v>
+        <v>433</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>430</v>
+        <v>434</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>431</v>
+        <v>435</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4164,16 +4188,16 @@
         <v>91</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>432</v>
+        <v>436</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>433</v>
+        <v>437</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>434</v>
+        <v>438</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>403</v>
+        <v>407</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4191,16 +4215,16 @@
         <v>104</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>435</v>
+        <v>439</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>436</v>
+        <v>440</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>437</v>
+        <v>441</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>438</v>
+        <v>442</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4211,16 +4235,16 @@
         <v>104</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>439</v>
+        <v>443</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>440</v>
+        <v>444</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>441</v>
+        <v>445</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>442</v>
+        <v>446</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4231,16 +4255,16 @@
         <v>104</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>443</v>
+        <v>447</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>444</v>
+        <v>448</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>446</v>
+        <v>450</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4251,16 +4275,16 @@
         <v>104</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>447</v>
+        <v>451</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>448</v>
+        <v>452</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>449</v>
+        <v>453</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>450</v>
+        <v>454</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4271,16 +4295,16 @@
         <v>104</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>451</v>
+        <v>455</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>452</v>
+        <v>456</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>453</v>
+        <v>457</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>454</v>
+        <v>458</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4295,16 +4319,16 @@
         <v>125</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>435</v>
+        <v>439</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>436</v>
+        <v>440</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>437</v>
+        <v>441</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>438</v>
+        <v>442</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4315,16 +4339,16 @@
         <v>125</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>439</v>
+        <v>443</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>440</v>
+        <v>444</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>441</v>
+        <v>445</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>442</v>
+        <v>446</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4335,16 +4359,16 @@
         <v>125</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>443</v>
+        <v>447</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>444</v>
+        <v>448</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>446</v>
+        <v>450</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4355,16 +4379,16 @@
         <v>125</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>447</v>
+        <v>451</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>448</v>
+        <v>452</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>449</v>
+        <v>453</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>450</v>
+        <v>454</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4375,16 +4399,16 @@
         <v>125</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>451</v>
+        <v>455</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>452</v>
+        <v>456</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>453</v>
+        <v>457</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>454</v>
+        <v>458</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Script update for Thunderbird LDA Keywords
</commit_message>
<xml_diff>
--- a/thesis-fine-grained-classification/binary-relevance/binary-relevance-meka-results.xlsx
+++ b/thesis-fine-grained-classification/binary-relevance/binary-relevance-meka-results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Lucene" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="858" uniqueCount="459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="874" uniqueCount="475">
   <si>
     <t xml:space="preserve">Model</t>
   </si>
@@ -1399,6 +1399,54 @@
   </si>
   <si>
     <t xml:space="preserve">0.820 0.876 0.934 0.950 0.981</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.534 0.420 0.119 0.209 0.728</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.622 0.615 0.667 0.061 0.944 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.376 0.268 0.063 0.118 0.573</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.789 0.867 0.934 0.852 0.981</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.718 0.727 0.672 0.740 0.751 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.429 0.291 0.148 0.156 0.623</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.806 0.812 0.614 0.704 0.607</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.687 0.681 0.734 0.775 0.968</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.654 0.574 0.318 0.476 0.784</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.586 0.520 0.271 0.348 0.697</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.521 0.415 0.190 0.316 0.650 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.791 0.857 0.910 0.930 0.973</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.430 0.273 0.100 0.076 0.721</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.558 0.474 0.476 0.375 0.930</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.279 0.159 0.053 0.039 0.564</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.767 0.850 0.932 0.944 0.980</t>
   </si>
 </sst>
 </file>
@@ -2577,7 +2625,7 @@
   </sheetPr>
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C47" activeCellId="0" sqref="C47"/>
     </sheetView>
   </sheetViews>
@@ -3653,8 +3701,8 @@
   </sheetPr>
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C47" activeCellId="0" sqref="C47"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C49" activeCellId="0" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -4418,6 +4466,18 @@
       <c r="B45" s="1" t="s">
         <v>126</v>
       </c>
+      <c r="C45" s="0" t="s">
+        <v>459</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>460</v>
+      </c>
+      <c r="E45" s="0" t="s">
+        <v>461</v>
+      </c>
+      <c r="F45" s="0" t="s">
+        <v>462</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
@@ -4426,6 +4486,18 @@
       <c r="B46" s="1" t="s">
         <v>126</v>
       </c>
+      <c r="C46" s="0" t="s">
+        <v>463</v>
+      </c>
+      <c r="D46" s="0" t="s">
+        <v>464</v>
+      </c>
+      <c r="E46" s="0" t="s">
+        <v>465</v>
+      </c>
+      <c r="F46" s="0" t="s">
+        <v>466</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
@@ -4434,6 +4506,18 @@
       <c r="B47" s="1" t="s">
         <v>126</v>
       </c>
+      <c r="C47" s="0" t="s">
+        <v>467</v>
+      </c>
+      <c r="D47" s="0" t="s">
+        <v>468</v>
+      </c>
+      <c r="E47" s="0" t="s">
+        <v>469</v>
+      </c>
+      <c r="F47" s="0" t="s">
+        <v>470</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
@@ -4441,6 +4525,18 @@
       </c>
       <c r="B48" s="1" t="s">
         <v>126</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>471</v>
+      </c>
+      <c r="D48" s="0" t="s">
+        <v>472</v>
+      </c>
+      <c r="E48" s="0" t="s">
+        <v>473</v>
+      </c>
+      <c r="F48" s="0" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Experimenting script for words in string matching using fuzzywuzzy
</commit_message>
<xml_diff>
--- a/thesis-fine-grained-classification/binary-relevance/binary-relevance-meka-results.xlsx
+++ b/thesis-fine-grained-classification/binary-relevance/binary-relevance-meka-results.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="874" uniqueCount="475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878" uniqueCount="479">
   <si>
     <t xml:space="preserve">Model</t>
   </si>
@@ -1447,6 +1447,18 @@
   </si>
   <si>
     <t xml:space="preserve">0.767 0.850 0.932 0.944 0.980</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.510 0.363 0.191 0.263 0.755</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.768 0.883 0.952 0.852 0.947</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.346 0.222 0.106 0.151 0.607</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.813 0.881 0.939 0.952 0.982</t>
   </si>
 </sst>
 </file>
@@ -3701,8 +3713,8 @@
   </sheetPr>
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C49" activeCellId="0" sqref="C49"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C53" activeCellId="0" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -4546,6 +4558,18 @@
       <c r="B49" s="1" t="s">
         <v>126</v>
       </c>
+      <c r="C49" s="0" t="s">
+        <v>475</v>
+      </c>
+      <c r="D49" s="0" t="s">
+        <v>476</v>
+      </c>
+      <c r="E49" s="0" t="s">
+        <v>477</v>
+      </c>
+      <c r="F49" s="0" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">

</xml_diff>

<commit_message>
Added results for fine grained classification Config 6 Binary Relevance Ubuntu
</commit_message>
<xml_diff>
--- a/thesis-fine-grained-classification/binary-relevance/binary-relevance-meka-results.xlsx
+++ b/thesis-fine-grained-classification/binary-relevance/binary-relevance-meka-results.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878" uniqueCount="479">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="505">
   <si>
     <t xml:space="preserve">Model</t>
   </si>
@@ -1459,6 +1459,84 @@
   </si>
   <si>
     <t xml:space="preserve">0.813 0.881 0.939 0.952 0.982</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.561 0.556 0.270 0.199 0.728</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.645 0.204 0.103 0.058 0.918 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.402 0.468 0.159 0.112 0.573</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.798 0.652 0.849 0.853 0.980</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.748 0.676 0.333 0.546 0.728</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.549 0.442 0.299 0.341 0.931</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.691 0.549 0.201 0.382 0.573</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.784 0.831 0.914 0.926 0.980 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.694 0.584 0.403 0.534 0.809</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.621 0.540 0.400 0.431 0.755 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.571 0.424 0.254 0.368 0.684</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.808 0.862 0.923 0.939 0.977 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.413 0.232 0.110 0.051 0.714</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.560 0.500 0.550 0.333 0.890</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.265 0.132 0.058 0.026 0.556</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.767 0.853 0.933 0.944 0.978</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.533 0.347 0.191 0.273 0.755</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.818 0.945 1.000 0.857 0.947</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.367 0.210 0.106 0.158 0.607</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.824 0.882 0.939 0.953 0.982</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.645 0.204 0.103 0.058 0.918</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.402 0.468 0.159 0.112 0.573 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.748 0.676 0.333 0.546 0.728 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.784 0.831 0.914 0.926 0.980</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.621 0.540 0.400 0.431 0.755</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.265 0.132 0.058 0.026 0.556 </t>
   </si>
 </sst>
 </file>
@@ -3714,7 +3792,7 @@
   <dimension ref="A1:F61"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C53" activeCellId="0" sqref="C53"/>
+      <selection pane="topLeft" activeCell="D63" activeCellId="0" sqref="D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -4578,6 +4656,18 @@
       <c r="B51" s="1" t="s">
         <v>147</v>
       </c>
+      <c r="C51" s="0" t="s">
+        <v>479</v>
+      </c>
+      <c r="D51" s="0" t="s">
+        <v>480</v>
+      </c>
+      <c r="E51" s="0" t="s">
+        <v>481</v>
+      </c>
+      <c r="F51" s="0" t="s">
+        <v>482</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
@@ -4586,6 +4676,18 @@
       <c r="B52" s="1" t="s">
         <v>147</v>
       </c>
+      <c r="C52" s="0" t="s">
+        <v>483</v>
+      </c>
+      <c r="D52" s="0" t="s">
+        <v>484</v>
+      </c>
+      <c r="E52" s="0" t="s">
+        <v>485</v>
+      </c>
+      <c r="F52" s="0" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
@@ -4594,6 +4696,18 @@
       <c r="B53" s="1" t="s">
         <v>147</v>
       </c>
+      <c r="C53" s="0" t="s">
+        <v>487</v>
+      </c>
+      <c r="D53" s="0" t="s">
+        <v>488</v>
+      </c>
+      <c r="E53" s="0" t="s">
+        <v>489</v>
+      </c>
+      <c r="F53" s="0" t="s">
+        <v>490</v>
+      </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
@@ -4602,6 +4716,18 @@
       <c r="B54" s="1" t="s">
         <v>147</v>
       </c>
+      <c r="C54" s="0" t="s">
+        <v>491</v>
+      </c>
+      <c r="D54" s="0" t="s">
+        <v>492</v>
+      </c>
+      <c r="E54" s="0" t="s">
+        <v>493</v>
+      </c>
+      <c r="F54" s="0" t="s">
+        <v>494</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
@@ -4610,6 +4736,18 @@
       <c r="B55" s="1" t="s">
         <v>147</v>
       </c>
+      <c r="C55" s="0" t="s">
+        <v>495</v>
+      </c>
+      <c r="D55" s="0" t="s">
+        <v>496</v>
+      </c>
+      <c r="E55" s="0" t="s">
+        <v>497</v>
+      </c>
+      <c r="F55" s="0" t="s">
+        <v>498</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
@@ -4618,6 +4756,18 @@
       <c r="B57" s="1" t="s">
         <v>168</v>
       </c>
+      <c r="C57" s="0" t="s">
+        <v>479</v>
+      </c>
+      <c r="D57" s="0" t="s">
+        <v>499</v>
+      </c>
+      <c r="E57" s="0" t="s">
+        <v>500</v>
+      </c>
+      <c r="F57" s="0" t="s">
+        <v>482</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
@@ -4626,6 +4776,18 @@
       <c r="B58" s="1" t="s">
         <v>168</v>
       </c>
+      <c r="C58" s="0" t="s">
+        <v>501</v>
+      </c>
+      <c r="D58" s="0" t="s">
+        <v>484</v>
+      </c>
+      <c r="E58" s="0" t="s">
+        <v>485</v>
+      </c>
+      <c r="F58" s="0" t="s">
+        <v>502</v>
+      </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
@@ -4634,6 +4796,18 @@
       <c r="B59" s="1" t="s">
         <v>168</v>
       </c>
+      <c r="C59" s="0" t="s">
+        <v>487</v>
+      </c>
+      <c r="D59" s="0" t="s">
+        <v>503</v>
+      </c>
+      <c r="E59" s="0" t="s">
+        <v>489</v>
+      </c>
+      <c r="F59" s="0" t="s">
+        <v>490</v>
+      </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
@@ -4642,6 +4816,18 @@
       <c r="B60" s="1" t="s">
         <v>168</v>
       </c>
+      <c r="C60" s="0" t="s">
+        <v>491</v>
+      </c>
+      <c r="D60" s="0" t="s">
+        <v>492</v>
+      </c>
+      <c r="E60" s="0" t="s">
+        <v>504</v>
+      </c>
+      <c r="F60" s="0" t="s">
+        <v>494</v>
+      </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
@@ -4649,6 +4835,18 @@
       </c>
       <c r="B61" s="1" t="s">
         <v>168</v>
+      </c>
+      <c r="C61" s="0" t="s">
+        <v>495</v>
+      </c>
+      <c r="D61" s="0" t="s">
+        <v>496</v>
+      </c>
+      <c r="E61" s="0" t="s">
+        <v>497</v>
+      </c>
+      <c r="F61" s="0" t="s">
+        <v>498</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Config 6 results for Label Powerset Dataset 1-3 Classifier 1-5
</commit_message>
<xml_diff>
--- a/thesis-fine-grained-classification/binary-relevance/binary-relevance-meka-results.xlsx
+++ b/thesis-fine-grained-classification/binary-relevance/binary-relevance-meka-results.xlsx
@@ -1639,19 +1639,19 @@
   </sheetPr>
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B47" activeCellId="0" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.9897959183673"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.0255102040816"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.1632653061224"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.5816326530612"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.6173469387755"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.9234693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.9795918367347"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2715,19 +2715,19 @@
   </sheetPr>
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C47" activeCellId="0" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.3979591836735"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.7295918367347"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.9948979591837"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.3214285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.0867346938776"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.2040816326531"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.3520408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3791,19 +3791,19 @@
   </sheetPr>
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D63" activeCellId="0" sqref="D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.1632653061224"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.0204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.2704081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.8571428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.6122448979592"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.8622448979592"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.7551020408163"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.234693877551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.4540816326531"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>